<commit_message>
Added view model measure to QAQC spreadsheet.
</commit_message>
<xml_diff>
--- a/projects/NECB_QA_QC.xlsx
+++ b/projects/NECB_QA_QC.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="565">
   <si>
     <t>type</t>
   </si>
@@ -1726,6 +1726,12 @@
   </si>
   <si>
     <t>GenericQAQC</t>
+  </si>
+  <si>
+    <t>ViewModel</t>
+  </si>
+  <si>
+    <t>view_model</t>
   </si>
 </sst>
 </file>
@@ -6178,7 +6184,27 @@
     <cellStyle name="Total" xfId="1817" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="1814" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -6264,8 +6290,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="7"/>
-      <tableStyleElement type="headerRow" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -7051,10 +7077,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7516,16 +7542,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>411</v>
+        <v>564</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>411</v>
+        <v>564</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>411</v>
+        <v>563</v>
       </c>
       <c r="E12" s="66" t="s">
-        <v>412</v>
+        <v>43</v>
       </c>
       <c r="F12" s="67"/>
       <c r="G12" s="67"/>
@@ -7541,28 +7567,58 @@
       <c r="Q12" s="67"/>
       <c r="R12" s="67"/>
     </row>
+    <row r="13" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>411</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>411</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>411</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>412</v>
+      </c>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="67"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:AA7"/>
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:A12">
-    <cfRule type="cellIs" dxfId="3" priority="84" operator="equal">
+  <conditionalFormatting sqref="A9:A13">
+    <cfRule type="cellIs" dxfId="5" priority="84" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A12">
-    <cfRule type="cellIs" dxfId="2" priority="83" operator="equal">
+  <conditionalFormatting sqref="A9:A13">
+    <cfRule type="cellIs" dxfId="4" priority="83" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="1" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="77" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="0" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="78" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added 3d viewer to output
</commit_message>
<xml_diff>
--- a/projects/NECB_QA_QC.xlsx
+++ b/projects/NECB_QA_QC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5550" windowWidth="20370" windowHeight="4965" tabRatio="469" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="5550" windowWidth="20370" windowHeight="4965" tabRatio="469" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="567">
   <si>
     <t>type</t>
   </si>
@@ -1732,6 +1732,12 @@
   </si>
   <si>
     <t>view_model</t>
+  </si>
+  <si>
+    <t>view_model.zipped_view_model_html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
   </si>
 </sst>
 </file>
@@ -7079,7 +7085,7 @@
   </sheetPr>
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -7629,11 +7635,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M285"/>
+  <dimension ref="A1:M286"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D265" sqref="D265"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C286" sqref="C286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13256,6 +13262,29 @@
         <v>1</v>
       </c>
       <c r="I285" s="58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A286" s="29" t="s">
+        <v>565</v>
+      </c>
+      <c r="B286" s="29" t="s">
+        <v>565</v>
+      </c>
+      <c r="D286" s="29" t="s">
+        <v>565</v>
+      </c>
+      <c r="F286" s="29" t="s">
+        <v>566</v>
+      </c>
+      <c r="G286" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H286" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I286" s="58" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified end use as per Meli's request
</commit_message>
<xml_diff>
--- a/projects/NECB_QA_QC.xlsx
+++ b/projects/NECB_QA_QC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5550" windowWidth="20370" windowHeight="4965" tabRatio="469" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="5550" windowWidth="20370" windowHeight="4965" tabRatio="469" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="601">
   <si>
     <t>type</t>
   </si>
@@ -1278,6 +1278,9 @@
     <t>ReportingMeasure</t>
   </si>
   <si>
+    <t>plopez</t>
+  </si>
+  <si>
     <t>%</t>
   </si>
   <si>
@@ -1689,24 +1692,12 @@
     <t>["FullServiceRestaurant","'Hospital'","HighriseApartment","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
   </si>
   <si>
-    <t>put_your_name_here</t>
-  </si>
-  <si>
     <t>1.20.1-nrcan</t>
   </si>
   <si>
-    <t>write_your_cluster_name_here</t>
-  </si>
-  <si>
     <t>write_your_analysis_name_here</t>
   </si>
   <si>
-    <t>["CAN_BC_Vancouver.718920_CWEC.epw"]</t>
-  </si>
-  <si>
-    <t>["FullServiceRestaurant","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
@@ -1738,6 +1729,117 @@
   </si>
   <si>
     <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VentilationQAQC </t>
+  </si>
+  <si>
+    <t>Phylroys_Cluster</t>
+  </si>
+  <si>
+    <t>["FullServiceRestaurant","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
+  </si>
+  <si>
+    <t>AdjustSystemEfficiencies</t>
+  </si>
+  <si>
+    <t>AdjustSystemEfficiencie</t>
+  </si>
+  <si>
+    <t>heating_efficiency_multiplier</t>
+  </si>
+  <si>
+    <t>[1.0]</t>
+  </si>
+  <si>
+    <t>cooling_cop_multiplier</t>
+  </si>
+  <si>
+    <t>../../OpenStudio-measures/NREL working measures</t>
+  </si>
+  <si>
+    <t>AdjustThermostatSetpointsByDegrees</t>
+  </si>
+  <si>
+    <t>cooling_adjustment</t>
+  </si>
+  <si>
+    <t>heating_adjustment</t>
+  </si>
+  <si>
+    <t>alter_design_days</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>[true]</t>
+  </si>
+  <si>
+    <t>[0.0]</t>
+  </si>
+  <si>
+    <t>AdjustWindowToWallRatios</t>
+  </si>
+  <si>
+    <t>wwr_multiplier</t>
+  </si>
+  <si>
+    <t>sillHeight</t>
+  </si>
+  <si>
+    <t>[30.0]</t>
+  </si>
+  <si>
+    <t>ImproveFanBeltEfficiency</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>motor_eff</t>
+  </si>
+  <si>
+    <t>*All Air Loops*</t>
+  </si>
+  <si>
+    <t>["*All Air Loops*"]</t>
+  </si>
+  <si>
+    <t>ImproveMotorEfficiency</t>
+  </si>
+  <si>
+    <t>*All Plant and Air Loops*</t>
+  </si>
+  <si>
+    <t>["*All Plant and Air Loops*"]</t>
+  </si>
+  <si>
+    <t>IncreaseInsulationRValueForExteriorWallsByPercentage</t>
+  </si>
+  <si>
+    <t>r_value</t>
+  </si>
+  <si>
+    <t>["0.0"]</t>
+  </si>
+  <si>
+    <t>IncreaseInsulationRValueForRoofsByPercentage</t>
+  </si>
+  <si>
+    <t>wall_r_value_percentage</t>
+  </si>
+  <si>
+    <t>roof_r_value_percentage</t>
+  </si>
+  <si>
+    <t>fan_motor_eff</t>
+  </si>
+  <si>
+    <t>fan_loops</t>
+  </si>
+  <si>
+    <t>motor_loops</t>
   </si>
 </sst>
 </file>
@@ -6190,7 +6292,17 @@
     <cellStyle name="Total" xfId="1817" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="1814" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="82">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -6224,6 +6336,716 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
       </font>
       <fill>
         <patternFill>
@@ -6296,8 +7118,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="9"/>
-      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="81"/>
+      <tableStyleElement type="headerRow" dxfId="80"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -6629,10 +7451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6679,7 +7501,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>550</v>
+        <v>413</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>67</v>
@@ -6696,12 +7518,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>552</v>
+        <v>565</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>80</v>
@@ -6772,7 +7594,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>79</v>
@@ -6802,122 +7624,130 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
+    <row r="15" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>22</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>183</v>
-      </c>
+        <v>572</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="29" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>91</v>
+        <v>72</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B20" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B21" s="28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="24"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:5" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B23" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>514</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>515</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B25" s="28">
         <v>2000</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C25" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="31"/>
-    </row>
     <row r="26" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
       <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6926,7 +7756,6 @@
     </row>
     <row r="29" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6934,65 +7763,61 @@
       <c r="C30" s="28"/>
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="28"/>
+    <row r="31" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="27"/>
       <c r="C31" s="28"/>
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="28"/>
       <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="28"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="D33" s="31"/>
+    </row>
+    <row r="34" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="28"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B35" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="D35" s="11"/>
+      <c r="E35" s="13"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B36" s="23" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="C36" s="29"/>
-    </row>
-    <row r="37" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="D37" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="C37" s="29"/>
     </row>
     <row r="38" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D38" s="2"/>
     </row>
@@ -7001,67 +7826,76 @@
         <v>26</v>
       </c>
       <c r="B39" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="41" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B42" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C42" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E42" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+    <row r="43" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C43" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D43" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+    <row r="45" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B45" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="13" t="s">
+      <c r="D45" s="11"/>
+      <c r="E45" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="C45" s="23"/>
-    </row>
-    <row r="46" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="24"/>
-      <c r="D46" s="2"/>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="29"/>
+      <c r="C46" s="23"/>
+    </row>
+    <row r="47" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="24"/>
+      <c r="D47" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
       <formula1>simulate_data_point</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7:B8">
@@ -7083,10 +7917,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7299,8 +8133,8 @@
       <c r="O5" s="64">
         <v>1</v>
       </c>
-      <c r="P5" s="62" t="s">
-        <v>555</v>
+      <c r="P5" s="44" t="s">
+        <v>566</v>
       </c>
       <c r="Q5" s="62"/>
       <c r="R5" s="62" t="s">
@@ -7431,8 +8265,8 @@
       <c r="O8" s="64">
         <v>1</v>
       </c>
-      <c r="P8" s="62" t="s">
-        <v>554</v>
+      <c r="P8" s="44" t="s">
+        <v>229</v>
       </c>
       <c r="Q8" s="62"/>
       <c r="R8" s="62" t="s">
@@ -7444,13 +8278,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="66" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D9" s="66" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E9" s="66" t="s">
         <v>43</v>
@@ -7474,13 +8308,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E10" s="66" t="s">
         <v>412</v>
@@ -7502,11 +8336,11 @@
     <row r="11" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" s="62" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C11" s="62"/>
       <c r="D11" s="62" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E11" s="62" t="s">
         <v>217</v>
@@ -7517,7 +8351,7 @@
       </c>
       <c r="H11" s="62"/>
       <c r="I11" s="70" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="J11" s="70"/>
       <c r="K11" s="62">
@@ -7536,7 +8370,7 @@
         <v>1</v>
       </c>
       <c r="P11" s="62" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="Q11" s="62"/>
       <c r="R11" s="62" t="s">
@@ -7548,13 +8382,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E12" s="66" t="s">
         <v>43</v>
@@ -7603,29 +8437,1021 @@
       <c r="Q13" s="67"/>
       <c r="R13" s="67"/>
     </row>
+    <row r="14" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="66" t="s">
+        <v>564</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>564</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>564</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>412</v>
+      </c>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="67"/>
+    </row>
+    <row r="15" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="66" t="s">
+        <v>567</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>567</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>568</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="67"/>
+    </row>
+    <row r="16" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="56"/>
+      <c r="B16" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62" t="s">
+        <v>569</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>569</v>
+      </c>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="62"/>
+      <c r="I16" s="70">
+        <v>1</v>
+      </c>
+      <c r="J16" s="70"/>
+      <c r="K16" s="62">
+        <v>1</v>
+      </c>
+      <c r="L16" s="62">
+        <v>1</v>
+      </c>
+      <c r="M16" s="62">
+        <v>1</v>
+      </c>
+      <c r="N16" s="62">
+        <v>1</v>
+      </c>
+      <c r="O16" s="62">
+        <v>1</v>
+      </c>
+      <c r="P16" s="62" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="56"/>
+      <c r="B17" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62" t="s">
+        <v>571</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>571</v>
+      </c>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="62"/>
+      <c r="I17" s="70">
+        <v>1</v>
+      </c>
+      <c r="J17" s="70"/>
+      <c r="K17" s="62">
+        <v>1</v>
+      </c>
+      <c r="L17" s="62">
+        <v>1</v>
+      </c>
+      <c r="M17" s="62">
+        <v>1</v>
+      </c>
+      <c r="N17" s="62">
+        <v>1</v>
+      </c>
+      <c r="O17" s="62">
+        <v>1</v>
+      </c>
+      <c r="P17" s="62" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" s="66" t="s">
+        <v>573</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>573</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>573</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="67"/>
+    </row>
+    <row r="19" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="56"/>
+      <c r="B19" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62" t="s">
+        <v>574</v>
+      </c>
+      <c r="E19" s="62" t="s">
+        <v>574</v>
+      </c>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="62"/>
+      <c r="I19" s="70">
+        <v>0</v>
+      </c>
+      <c r="J19" s="70"/>
+      <c r="K19" s="62">
+        <v>0</v>
+      </c>
+      <c r="L19" s="62">
+        <v>0</v>
+      </c>
+      <c r="M19" s="62">
+        <v>0</v>
+      </c>
+      <c r="N19" s="62">
+        <v>0</v>
+      </c>
+      <c r="O19" s="62">
+        <v>0</v>
+      </c>
+      <c r="P19" s="62" t="s">
+        <v>579</v>
+      </c>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="56"/>
+      <c r="B20" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62" t="s">
+        <v>575</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>575</v>
+      </c>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="62"/>
+      <c r="I20" s="70">
+        <v>0</v>
+      </c>
+      <c r="J20" s="70"/>
+      <c r="K20" s="62">
+        <v>0</v>
+      </c>
+      <c r="L20" s="62">
+        <v>0</v>
+      </c>
+      <c r="M20" s="62">
+        <v>0</v>
+      </c>
+      <c r="N20" s="62">
+        <v>0</v>
+      </c>
+      <c r="O20" s="62">
+        <v>0</v>
+      </c>
+      <c r="P20" s="62" t="s">
+        <v>579</v>
+      </c>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="56"/>
+      <c r="B21" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62" t="s">
+        <v>576</v>
+      </c>
+      <c r="E21" s="62" t="s">
+        <v>576</v>
+      </c>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62" t="s">
+        <v>577</v>
+      </c>
+      <c r="H21" s="62"/>
+      <c r="I21" s="70" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="70"/>
+      <c r="K21" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" s="62" t="s">
+        <v>578</v>
+      </c>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B22" s="66" t="s">
+        <v>580</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>580</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>580</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+    </row>
+    <row r="23" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="56"/>
+      <c r="B23" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62" t="s">
+        <v>581</v>
+      </c>
+      <c r="E23" s="62" t="s">
+        <v>581</v>
+      </c>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="62"/>
+      <c r="I23" s="70">
+        <v>1</v>
+      </c>
+      <c r="J23" s="70"/>
+      <c r="K23" s="62">
+        <v>1</v>
+      </c>
+      <c r="L23" s="62">
+        <v>1</v>
+      </c>
+      <c r="M23" s="62">
+        <v>1</v>
+      </c>
+      <c r="N23" s="62">
+        <v>1</v>
+      </c>
+      <c r="O23" s="62">
+        <v>1</v>
+      </c>
+      <c r="P23" s="62" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="56"/>
+      <c r="B24" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62" t="s">
+        <v>582</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>582</v>
+      </c>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="62"/>
+      <c r="I24" s="70">
+        <v>30</v>
+      </c>
+      <c r="J24" s="70"/>
+      <c r="K24" s="62">
+        <v>30</v>
+      </c>
+      <c r="L24" s="62">
+        <v>30</v>
+      </c>
+      <c r="M24" s="62">
+        <v>30</v>
+      </c>
+      <c r="N24" s="62">
+        <v>30</v>
+      </c>
+      <c r="O24" s="62">
+        <v>30</v>
+      </c>
+      <c r="P24" s="62" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q24" s="62"/>
+      <c r="R24" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" s="66" t="s">
+        <v>584</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>584</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>584</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="67"/>
+    </row>
+    <row r="26" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="56"/>
+      <c r="B26" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62" t="s">
+        <v>599</v>
+      </c>
+      <c r="E26" s="62" t="s">
+        <v>585</v>
+      </c>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="H26" s="62"/>
+      <c r="I26" s="70" t="s">
+        <v>587</v>
+      </c>
+      <c r="J26" s="70"/>
+      <c r="K26" s="62">
+        <v>1</v>
+      </c>
+      <c r="L26" s="62">
+        <v>1</v>
+      </c>
+      <c r="M26" s="62">
+        <v>1</v>
+      </c>
+      <c r="N26" s="62">
+        <v>1</v>
+      </c>
+      <c r="O26" s="62">
+        <v>1</v>
+      </c>
+      <c r="P26" s="62" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q26" s="62"/>
+      <c r="R26" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="56"/>
+      <c r="B27" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62" t="s">
+        <v>598</v>
+      </c>
+      <c r="E27" s="62" t="s">
+        <v>586</v>
+      </c>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="62"/>
+      <c r="I27" s="70">
+        <v>1</v>
+      </c>
+      <c r="J27" s="70"/>
+      <c r="K27" s="62">
+        <v>1</v>
+      </c>
+      <c r="L27" s="62">
+        <v>1</v>
+      </c>
+      <c r="M27" s="62">
+        <v>1</v>
+      </c>
+      <c r="N27" s="62">
+        <v>1</v>
+      </c>
+      <c r="O27" s="62">
+        <v>1</v>
+      </c>
+      <c r="P27" s="62" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" s="66" t="s">
+        <v>589</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>589</v>
+      </c>
+      <c r="D28" s="66" t="s">
+        <v>589</v>
+      </c>
+      <c r="E28" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="67"/>
+      <c r="P28" s="67"/>
+      <c r="Q28" s="67"/>
+      <c r="R28" s="67"/>
+    </row>
+    <row r="29" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="56"/>
+      <c r="B29" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62" t="s">
+        <v>600</v>
+      </c>
+      <c r="E29" s="62" t="s">
+        <v>585</v>
+      </c>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="H29" s="62"/>
+      <c r="I29" s="70" t="s">
+        <v>590</v>
+      </c>
+      <c r="J29" s="70"/>
+      <c r="K29" s="62">
+        <v>1</v>
+      </c>
+      <c r="L29" s="62">
+        <v>1</v>
+      </c>
+      <c r="M29" s="62">
+        <v>1</v>
+      </c>
+      <c r="N29" s="62">
+        <v>1</v>
+      </c>
+      <c r="O29" s="62">
+        <v>1</v>
+      </c>
+      <c r="P29" s="62" t="s">
+        <v>591</v>
+      </c>
+      <c r="Q29" s="62"/>
+      <c r="R29" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="56"/>
+      <c r="B30" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62" t="s">
+        <v>586</v>
+      </c>
+      <c r="E30" s="62" t="s">
+        <v>586</v>
+      </c>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="62"/>
+      <c r="I30" s="70">
+        <v>1</v>
+      </c>
+      <c r="J30" s="70"/>
+      <c r="K30" s="62">
+        <v>1</v>
+      </c>
+      <c r="L30" s="62">
+        <v>1</v>
+      </c>
+      <c r="M30" s="62">
+        <v>1</v>
+      </c>
+      <c r="N30" s="62">
+        <v>1</v>
+      </c>
+      <c r="O30" s="62">
+        <v>1</v>
+      </c>
+      <c r="P30" s="62" t="s">
+        <v>570</v>
+      </c>
+      <c r="Q30" s="62"/>
+      <c r="R30" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B31" s="66" t="s">
+        <v>592</v>
+      </c>
+      <c r="C31" s="66" t="s">
+        <v>592</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>592</v>
+      </c>
+      <c r="E31" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="67"/>
+    </row>
+    <row r="32" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62" t="s">
+        <v>596</v>
+      </c>
+      <c r="E32" s="62" t="s">
+        <v>593</v>
+      </c>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="H32" s="62"/>
+      <c r="I32" s="70">
+        <v>0</v>
+      </c>
+      <c r="J32" s="70"/>
+      <c r="K32" s="62">
+        <v>0</v>
+      </c>
+      <c r="L32" s="62">
+        <v>0</v>
+      </c>
+      <c r="M32" s="62">
+        <v>0</v>
+      </c>
+      <c r="N32" s="62">
+        <v>0</v>
+      </c>
+      <c r="O32" s="62">
+        <v>0</v>
+      </c>
+      <c r="P32" s="62" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q32" s="62"/>
+      <c r="R32" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="66" t="s">
+        <v>595</v>
+      </c>
+      <c r="C33" s="66" t="s">
+        <v>595</v>
+      </c>
+      <c r="D33" s="66" t="s">
+        <v>595</v>
+      </c>
+      <c r="E33" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="67"/>
+      <c r="P33" s="67"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="67"/>
+    </row>
+    <row r="34" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="56"/>
+      <c r="B34" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62" t="s">
+        <v>597</v>
+      </c>
+      <c r="E34" s="62" t="s">
+        <v>593</v>
+      </c>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="H34" s="62"/>
+      <c r="I34" s="70">
+        <v>0</v>
+      </c>
+      <c r="J34" s="70"/>
+      <c r="K34" s="62">
+        <v>0</v>
+      </c>
+      <c r="L34" s="62">
+        <v>0</v>
+      </c>
+      <c r="M34" s="62">
+        <v>0</v>
+      </c>
+      <c r="N34" s="62">
+        <v>0</v>
+      </c>
+      <c r="O34" s="62">
+        <v>0</v>
+      </c>
+      <c r="P34" s="62" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q34" s="62"/>
+      <c r="R34" s="62" t="s">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:AA7"/>
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:A13">
-    <cfRule type="cellIs" dxfId="5" priority="84" operator="equal">
+  <conditionalFormatting sqref="A9:A15">
+    <cfRule type="cellIs" dxfId="47" priority="122" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A13">
-    <cfRule type="cellIs" dxfId="4" priority="83" operator="equal">
+  <conditionalFormatting sqref="A9:A15">
+    <cfRule type="cellIs" dxfId="46" priority="121" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="3" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="115" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="2" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="116" operator="equal">
       <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:A21">
+    <cfRule type="cellIs" dxfId="43" priority="29" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="cellIs" dxfId="41" priority="37" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="cellIs" dxfId="40" priority="23" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:A21">
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7637,7 +9463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M286"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C286" sqref="C286"/>
     </sheetView>
@@ -11240,14 +13066,14 @@
     </row>
     <row r="198" spans="1:13" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="54" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B198" s="54" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C198" s="54"/>
       <c r="D198" s="54" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E198" s="54"/>
       <c r="F198" s="54" t="s">
@@ -11269,13 +13095,13 @@
     </row>
     <row r="199" spans="1:13" s="5" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D199" s="5" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F199" s="55" t="s">
         <v>41</v>
@@ -11292,16 +13118,16 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="29" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B200" s="29" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F200" s="29" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="G200" s="58" t="b">
         <v>1</v>
@@ -11315,16 +13141,16 @@
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="29" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B201" s="29" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D201" s="29" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F201" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G201" s="58" t="b">
         <v>1</v>
@@ -11338,16 +13164,16 @@
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="29" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B202" s="29" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D202" s="29" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F202" s="29" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G202" s="58" t="b">
         <v>1</v>
@@ -11361,16 +13187,16 @@
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="29" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B203" s="29" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F203" s="29" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G203" s="58" t="b">
         <v>1</v>
@@ -11384,16 +13210,16 @@
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="29" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B204" s="29" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F204" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G204" s="58" t="b">
         <v>1</v>
@@ -11407,16 +13233,16 @@
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B205" s="29" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F205" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G205" s="58" t="b">
         <v>1</v>
@@ -11430,16 +13256,16 @@
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="29" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B206" s="29" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D206" s="29" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F206" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G206" s="58" t="b">
         <v>1</v>
@@ -11453,16 +13279,16 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="29" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B207" s="29" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F207" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G207" s="58" t="b">
         <v>1</v>
@@ -11476,16 +13302,16 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="29" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B208" s="29" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F208" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G208" s="58" t="b">
         <v>1</v>
@@ -11499,16 +13325,16 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="29" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B209" s="29" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F209" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G209" s="58" t="b">
         <v>1</v>
@@ -11522,16 +13348,16 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="29" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B210" s="29" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F210" s="29" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="G210" s="58" t="b">
         <v>1</v>
@@ -11545,16 +13371,16 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="29" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B211" s="29" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F211" s="29" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="G211" s="58" t="b">
         <v>1</v>
@@ -11568,16 +13394,16 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="29" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B212" s="29" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F212" s="29" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G212" s="58" t="b">
         <v>1</v>
@@ -11591,16 +13417,16 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="29" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B213" s="29" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F213" s="29" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G213" s="58" t="b">
         <v>1</v>
@@ -11614,16 +13440,16 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="29" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B214" s="29" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F214" s="29" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="G214" s="58" t="b">
         <v>1</v>
@@ -11637,16 +13463,16 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="29" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B215" s="29" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F215" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G215" s="58" t="b">
         <v>1</v>
@@ -11660,16 +13486,16 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="29" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B216" s="29" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F216" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G216" s="58" t="b">
         <v>1</v>
@@ -11683,16 +13509,16 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="29" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B217" s="29" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F217" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G217" s="58" t="b">
         <v>1</v>
@@ -11706,16 +13532,16 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="29" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B218" s="29" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F218" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G218" s="58" t="b">
         <v>1</v>
@@ -11729,16 +13555,16 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="29" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B219" s="29" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F219" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G219" s="58" t="b">
         <v>1</v>
@@ -11752,16 +13578,16 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="29" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B220" s="29" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F220" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G220" s="58" t="b">
         <v>1</v>
@@ -11775,16 +13601,16 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="29" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B221" s="29" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F221" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G221" s="58" t="b">
         <v>1</v>
@@ -11798,16 +13624,16 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="29" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B222" s="29" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D222" s="29" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F222" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G222" s="58" t="b">
         <v>1</v>
@@ -11821,16 +13647,16 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="29" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B223" s="29" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D223" s="29" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F223" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G223" s="58" t="b">
         <v>1</v>
@@ -11844,16 +13670,16 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="29" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B224" s="29" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D224" s="29" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F224" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G224" s="58" t="b">
         <v>1</v>
@@ -11867,16 +13693,16 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="29" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B225" s="29" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D225" s="29" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F225" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G225" s="58" t="b">
         <v>1</v>
@@ -11890,16 +13716,16 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="29" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B226" s="29" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D226" s="29" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F226" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G226" s="58" t="b">
         <v>1</v>
@@ -11913,16 +13739,16 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="29" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B227" s="29" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D227" s="29" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F227" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G227" s="58" t="b">
         <v>1</v>
@@ -11936,16 +13762,16 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="29" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B228" s="29" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D228" s="29" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="F228" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G228" s="58" t="b">
         <v>1</v>
@@ -11959,16 +13785,16 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="29" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B229" s="29" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D229" s="29" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F229" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G229" s="58" t="b">
         <v>1</v>
@@ -11982,16 +13808,16 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="29" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B230" s="29" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D230" s="29" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F230" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G230" s="58" t="b">
         <v>1</v>
@@ -12005,16 +13831,16 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="29" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B231" s="29" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D231" s="29" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F231" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G231" s="58" t="b">
         <v>1</v>
@@ -12028,16 +13854,16 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="29" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B232" s="29" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D232" s="29" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F232" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G232" s="58" t="b">
         <v>1</v>
@@ -12051,16 +13877,16 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="29" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B233" s="29" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D233" s="29" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F233" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G233" s="58" t="b">
         <v>1</v>
@@ -12074,16 +13900,16 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="29" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B234" s="29" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D234" s="29" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F234" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G234" s="58" t="b">
         <v>1</v>
@@ -12097,16 +13923,16 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="29" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B235" s="29" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D235" s="29" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="F235" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G235" s="58" t="b">
         <v>1</v>
@@ -12120,16 +13946,16 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="29" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B236" s="29" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D236" s="29" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F236" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G236" s="58" t="b">
         <v>1</v>
@@ -12143,16 +13969,16 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="29" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B237" s="29" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D237" s="29" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F237" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G237" s="58" t="b">
         <v>1</v>
@@ -12166,16 +13992,16 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="29" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B238" s="29" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D238" s="29" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F238" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G238" s="58" t="b">
         <v>1</v>
@@ -12189,16 +14015,16 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="29" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B239" s="29" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D239" s="29" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F239" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G239" s="58" t="b">
         <v>1</v>
@@ -12212,16 +14038,16 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="29" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B240" s="29" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D240" s="29" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F240" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G240" s="58" t="b">
         <v>1</v>
@@ -12235,16 +14061,16 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="29" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B241" s="29" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D241" s="29" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F241" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G241" s="58" t="b">
         <v>1</v>
@@ -12258,16 +14084,16 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="29" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B242" s="29" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D242" s="29" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F242" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G242" s="58" t="b">
         <v>1</v>
@@ -12281,16 +14107,16 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="29" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B243" s="29" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D243" s="29" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="F243" s="29" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="G243" s="58" t="b">
         <v>1</v>
@@ -12304,16 +14130,16 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="29" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B244" s="29" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D244" s="29" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="F244" s="29" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="G244" s="58" t="b">
         <v>1</v>
@@ -12327,16 +14153,16 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="29" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B245" s="29" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D245" s="29" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F245" s="29" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G245" s="58" t="b">
         <v>1</v>
@@ -12350,16 +14176,16 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="29" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B246" s="29" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D246" s="29" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F246" s="29" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G246" s="58" t="b">
         <v>1</v>
@@ -12373,16 +14199,16 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="29" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B247" s="29" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D247" s="29" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F247" s="29" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G247" s="58" t="b">
         <v>1</v>
@@ -12396,16 +14222,16 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="29" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B248" s="29" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D248" s="29" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F248" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G248" s="58" t="b">
         <v>1</v>
@@ -12419,16 +14245,16 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="29" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B249" s="29" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D249" s="29" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F249" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G249" s="58" t="b">
         <v>1</v>
@@ -12442,16 +14268,16 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="29" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B250" s="29" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D250" s="29" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F250" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G250" s="58" t="b">
         <v>1</v>
@@ -12465,16 +14291,16 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="29" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B251" s="29" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D251" s="29" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F251" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G251" s="58" t="b">
         <v>1</v>
@@ -12488,16 +14314,16 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="29" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B252" s="29" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D252" s="29" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F252" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G252" s="58" t="b">
         <v>1</v>
@@ -12511,16 +14337,16 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="29" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B253" s="29" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D253" s="29" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F253" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G253" s="58" t="b">
         <v>1</v>
@@ -12534,16 +14360,16 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="29" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B254" s="29" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D254" s="29" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F254" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G254" s="58" t="b">
         <v>1</v>
@@ -12557,16 +14383,16 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="29" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B255" s="29" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D255" s="29" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F255" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G255" s="58" t="b">
         <v>1</v>
@@ -12580,16 +14406,16 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="29" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B256" s="29" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D256" s="29" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F256" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G256" s="58" t="b">
         <v>1</v>
@@ -12603,16 +14429,16 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="29" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B257" s="29" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D257" s="29" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F257" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G257" s="58" t="b">
         <v>1</v>
@@ -12626,16 +14452,16 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="29" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D258" s="29" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F258" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G258" s="58" t="b">
         <v>1</v>
@@ -12649,16 +14475,16 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="29" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B259" s="29" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D259" s="29" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F259" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G259" s="58" t="b">
         <v>1</v>
@@ -12672,16 +14498,16 @@
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="29" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B260" s="29" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D260" s="29" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F260" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G260" s="58" t="b">
         <v>1</v>
@@ -12695,16 +14521,16 @@
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="29" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B261" s="29" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D261" s="29" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F261" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G261" s="58" t="b">
         <v>1</v>
@@ -12718,16 +14544,16 @@
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="29" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B262" s="29" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D262" s="29" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F262" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G262" s="58" t="b">
         <v>1</v>
@@ -12741,16 +14567,16 @@
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="29" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B263" s="29" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D263" s="29" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F263" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G263" s="58" t="b">
         <v>1</v>
@@ -12764,16 +14590,16 @@
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="29" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B264" s="29" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D264" s="29" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F264" s="29" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G264" s="58" t="b">
         <v>1</v>
@@ -12787,16 +14613,16 @@
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="29" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B265" s="29" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D265" s="29" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F265" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G265" s="58" t="b">
         <v>1</v>
@@ -12810,16 +14636,16 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="29" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B266" s="29" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D266" s="29" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="F266" s="29" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="G266" s="58" t="b">
         <v>1</v>
@@ -12833,16 +14659,16 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="29" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B267" s="29" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D267" s="29" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F267" s="29" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="G267" s="58" t="b">
         <v>1</v>
@@ -12856,13 +14682,13 @@
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="29" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B268" s="29" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D268" s="29" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="G268" s="58" t="b">
         <v>1</v>
@@ -12876,16 +14702,16 @@
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="29" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B269" s="29" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D269" s="29" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F269" s="29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G269" s="58" t="b">
         <v>1</v>
@@ -12899,16 +14725,16 @@
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="29" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B270" s="29" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D270" s="29" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F270" s="29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G270" s="58" t="b">
         <v>1</v>
@@ -12922,16 +14748,16 @@
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="29" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B271" s="29" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D271" s="29" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F271" s="29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G271" s="58" t="b">
         <v>1</v>
@@ -12945,16 +14771,16 @@
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="29" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B272" s="29" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D272" s="29" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F272" s="29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G272" s="58" t="b">
         <v>1</v>
@@ -12968,16 +14794,16 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="29" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B273" s="29" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D273" s="29" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F273" s="29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G273" s="58" t="b">
         <v>1</v>
@@ -12991,16 +14817,16 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="29" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B274" s="29" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D274" s="29" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F274" s="29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G274" s="58" t="b">
         <v>1</v>
@@ -13014,16 +14840,16 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="29" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B275" s="29" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D275" s="29" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F275" s="29" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G275" s="58" t="b">
         <v>1</v>
@@ -13037,16 +14863,16 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="29" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B276" s="29" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D276" s="29" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F276" s="29" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G276" s="58" t="b">
         <v>1</v>
@@ -13060,16 +14886,16 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="29" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B277" s="29" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D277" s="29" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F277" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G277" s="58" t="b">
         <v>1</v>
@@ -13083,16 +14909,16 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="29" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B278" s="29" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D278" s="29" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F278" s="29" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G278" s="58" t="b">
         <v>1</v>
@@ -13106,16 +14932,16 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="29" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B279" s="29" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D279" s="29" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F279" s="29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G279" s="58" t="b">
         <v>1</v>
@@ -13129,16 +14955,16 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="29" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B280" s="29" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D280" s="29" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F280" s="29" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G280" s="58" t="b">
         <v>1</v>
@@ -13152,16 +14978,16 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="29" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B281" s="29" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D281" s="29" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F281" s="29" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G281" s="58" t="b">
         <v>1</v>
@@ -13175,16 +15001,16 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" s="29" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B282" s="29" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D282" s="29" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="F282" s="29" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G282" s="58" t="b">
         <v>1</v>
@@ -13198,16 +15024,16 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="29" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B283" s="29" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D283" s="29" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F283" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G283" s="58" t="b">
         <v>1</v>
@@ -13221,16 +15047,16 @@
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="29" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B284" s="29" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D284" s="29" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="F284" s="29" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="G284" s="58" t="b">
         <v>1</v>
@@ -13244,16 +15070,16 @@
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" s="29" t="s">
+        <v>549</v>
+      </c>
+      <c r="B285" s="29" t="s">
+        <v>549</v>
+      </c>
+      <c r="D285" s="29" t="s">
+        <v>549</v>
+      </c>
+      <c r="F285" s="29" t="s">
         <v>548</v>
-      </c>
-      <c r="B285" s="29" t="s">
-        <v>548</v>
-      </c>
-      <c r="D285" s="29" t="s">
-        <v>548</v>
-      </c>
-      <c r="F285" s="29" t="s">
-        <v>547</v>
       </c>
       <c r="G285" s="58" t="b">
         <v>1</v>
@@ -13267,16 +15093,16 @@
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" s="29" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B286" s="29" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D286" s="29" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F286" s="29" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="G286" s="58" t="b">
         <v>1</v>
@@ -13805,7 +15631,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13815,15 +15641,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B2" t="s">
         <v>229</v>
@@ -13834,106 +15660,106 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B4" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B5" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B6" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B7" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B8" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B10" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B11" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B12" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B13" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B14" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B15" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B16" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -13944,10 +15770,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="59" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B19" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added measures to QAQC project
</commit_message>
<xml_diff>
--- a/projects/NECB_QA_QC.xlsx
+++ b/projects/NECB_QA_QC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5550" windowWidth="20370" windowHeight="4965" tabRatio="469" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="5610" windowWidth="20370" windowHeight="4905" tabRatio="469" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="610">
   <si>
     <t>type</t>
   </si>
@@ -1737,15 +1737,9 @@
     <t>Phylroys_Cluster</t>
   </si>
   <si>
-    <t>["FullServiceRestaurant","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
-  </si>
-  <si>
     <t>AdjustSystemEfficiencies</t>
   </si>
   <si>
-    <t>AdjustSystemEfficiencie</t>
-  </si>
-  <si>
     <t>heating_efficiency_multiplier</t>
   </si>
   <si>
@@ -1821,9 +1815,6 @@
     <t>r_value</t>
   </si>
   <si>
-    <t>["0.0"]</t>
-  </si>
-  <si>
     <t>IncreaseInsulationRValueForRoofsByPercentage</t>
   </si>
   <si>
@@ -1840,6 +1831,42 @@
   </si>
   <si>
     <t>motor_loops</t>
+  </si>
+  <si>
+    <t>[-0.5,-0.25,0.0,0.25,0.5]</t>
+  </si>
+  <si>
+    <t>["LargeOffice",]</t>
+  </si>
+  <si>
+    <t>["CAN_ON_Toronto.716240_CWEC.epw"]</t>
+  </si>
+  <si>
+    <t>[-75.0,-25.0,0.0,25.0,75.0]</t>
+  </si>
+  <si>
+    <t>[0.5, 1.0, 1.2]</t>
+  </si>
+  <si>
+    <t>ReduceSpaceInfiltrationByPercentage</t>
+  </si>
+  <si>
+    <t>space_type</t>
+  </si>
+  <si>
+    <t>space_infiltration_reduction_percent</t>
+  </si>
+  <si>
+    <t>[-50.0,-25.0,0.0,25.0]</t>
+  </si>
+  <si>
+    <t>["*Entire Building*"]</t>
+  </si>
+  <si>
+    <t>infiltration_space_type</t>
+  </si>
+  <si>
+    <t>[0.75,1.0,1.1,1.15]</t>
   </si>
 </sst>
 </file>
@@ -4432,9 +4459,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4447,6 +4471,9 @@
     <xf numFmtId="0" fontId="28" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1842">
     <cellStyle name="20% - Accent1" xfId="1819" builtinId="30" customBuiltin="1"/>
@@ -6292,7 +6319,27 @@
     <cellStyle name="Total" xfId="1817" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="1814" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="52">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -6345,7 +6392,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </font>
       <fill>
         <patternFill>
@@ -6355,7 +6402,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill>
@@ -6775,326 +6822,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -7118,8 +6845,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="81"/>
-      <tableStyleElement type="headerRow" dxfId="80"/>
+      <tableStyleElement type="wholeTable" dxfId="51"/>
+      <tableStyleElement type="headerRow" dxfId="50"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -7454,7 +7181,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7534,34 +7261,34 @@
         <v>52</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C7" s="30" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
-        <v xml:space="preserve">2 Cores - Worker Only - </v>
+        <v>4 Cores - Recommended for Server</v>
       </c>
       <c r="D7" s="30" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
-        <v>$0.11/hour</v>
+        <v>$0.28/hour</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C8" s="30" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
-        <v xml:space="preserve">4 Cores - Worker Only - </v>
+        <v>16 Cores - Worker Only - Recommended for Worker</v>
       </c>
       <c r="D8" s="30" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
-        <v>$0.21/hour</v>
+        <v>$1.68/hour</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>54</v>
@@ -7629,7 +7356,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="29" t="s">
@@ -7730,7 +7457,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="28">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>135</v>
@@ -7917,10 +7644,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7975,14 +7702,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -8099,281 +7826,281 @@
     </row>
     <row r="5" spans="1:26" s="48" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57"/>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="61" t="s">
         <v>208</v>
       </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62" t="s">
+      <c r="F5" s="61"/>
+      <c r="G5" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62" t="s">
+      <c r="H5" s="61"/>
+      <c r="I5" s="61" t="s">
         <v>220</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="64">
-        <v>1</v>
-      </c>
-      <c r="L5" s="64">
-        <v>1</v>
-      </c>
-      <c r="M5" s="64">
-        <v>1</v>
-      </c>
-      <c r="N5" s="64">
-        <v>1</v>
-      </c>
-      <c r="O5" s="64">
+      <c r="J5" s="62"/>
+      <c r="K5" s="63">
+        <v>1</v>
+      </c>
+      <c r="L5" s="63">
+        <v>1</v>
+      </c>
+      <c r="M5" s="63">
+        <v>1</v>
+      </c>
+      <c r="N5" s="63">
+        <v>1</v>
+      </c>
+      <c r="O5" s="63">
         <v>1</v>
       </c>
       <c r="P5" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="48" customFormat="1" ht="14.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="57"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62" t="s">
+      <c r="C6" s="61"/>
+      <c r="D6" s="61" t="s">
         <v>209</v>
       </c>
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62" t="s">
+      <c r="F6" s="61"/>
+      <c r="G6" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62" t="s">
+      <c r="H6" s="61"/>
+      <c r="I6" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="J6" s="62"/>
-      <c r="K6" s="64">
-        <v>1</v>
-      </c>
-      <c r="L6" s="64">
-        <v>1</v>
-      </c>
-      <c r="M6" s="64">
-        <v>1</v>
-      </c>
-      <c r="N6" s="64">
-        <v>1</v>
-      </c>
-      <c r="O6" s="64">
-        <v>1</v>
-      </c>
-      <c r="P6" s="62" t="s">
+      <c r="J6" s="61"/>
+      <c r="K6" s="63">
+        <v>1</v>
+      </c>
+      <c r="L6" s="63">
+        <v>1</v>
+      </c>
+      <c r="M6" s="63">
+        <v>1</v>
+      </c>
+      <c r="N6" s="63">
+        <v>1</v>
+      </c>
+      <c r="O6" s="63">
+        <v>1</v>
+      </c>
+      <c r="P6" s="61" t="s">
         <v>222</v>
       </c>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62" t="s">
+      <c r="Q6" s="61"/>
+      <c r="R6" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="48" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="57"/>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62" t="s">
+      <c r="C7" s="61"/>
+      <c r="D7" s="61" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="61"/>
+      <c r="G7" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="65" t="s">
+      <c r="H7" s="61"/>
+      <c r="I7" s="64" t="s">
         <v>223</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="64">
-        <v>1</v>
-      </c>
-      <c r="L7" s="64">
-        <v>1</v>
-      </c>
-      <c r="M7" s="64">
-        <v>1</v>
-      </c>
-      <c r="N7" s="64">
-        <v>1</v>
-      </c>
-      <c r="O7" s="64">
-        <v>1</v>
-      </c>
-      <c r="P7" s="65" t="s">
+      <c r="J7" s="61"/>
+      <c r="K7" s="63">
+        <v>1</v>
+      </c>
+      <c r="L7" s="63">
+        <v>1</v>
+      </c>
+      <c r="M7" s="63">
+        <v>1</v>
+      </c>
+      <c r="N7" s="63">
+        <v>1</v>
+      </c>
+      <c r="O7" s="63">
+        <v>1</v>
+      </c>
+      <c r="P7" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62" t="s">
+      <c r="Q7" s="61"/>
+      <c r="R7" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="48" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="57"/>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61" t="s">
         <v>225</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="61" t="s">
         <v>226</v>
       </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62" t="s">
+      <c r="F8" s="61"/>
+      <c r="G8" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="H8" s="62"/>
-      <c r="I8" s="65" t="s">
+      <c r="H8" s="61"/>
+      <c r="I8" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="J8" s="62"/>
-      <c r="K8" s="64">
-        <v>1</v>
-      </c>
-      <c r="L8" s="64">
-        <v>1</v>
-      </c>
-      <c r="M8" s="64">
-        <v>1</v>
-      </c>
-      <c r="N8" s="64">
-        <v>1</v>
-      </c>
-      <c r="O8" s="64">
+      <c r="J8" s="61"/>
+      <c r="K8" s="63">
+        <v>1</v>
+      </c>
+      <c r="L8" s="63">
+        <v>1</v>
+      </c>
+      <c r="M8" s="63">
+        <v>1</v>
+      </c>
+      <c r="N8" s="63">
+        <v>1</v>
+      </c>
+      <c r="O8" s="63">
         <v>1</v>
       </c>
       <c r="P8" s="44" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="66" t="s">
+    <row r="9" spans="1:26" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="68" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="65" t="s">
         <v>553</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="65" t="s">
         <v>553</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="65" t="s">
         <v>553</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="67"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
     </row>
     <row r="10" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>554</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>554</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="65" t="s">
         <v>559</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="65" t="s">
         <v>412</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
     </row>
     <row r="11" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>555</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62" t="s">
+      <c r="C11" s="61"/>
+      <c r="D11" s="61" t="s">
         <v>556</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62" t="s">
+      <c r="F11" s="61"/>
+      <c r="G11" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="70" t="s">
+      <c r="H11" s="61"/>
+      <c r="I11" s="69" t="s">
         <v>557</v>
       </c>
-      <c r="J11" s="70"/>
-      <c r="K11" s="62">
-        <v>1</v>
-      </c>
-      <c r="L11" s="62">
-        <v>1</v>
-      </c>
-      <c r="M11" s="62">
-        <v>1</v>
-      </c>
-      <c r="N11" s="62">
-        <v>1</v>
-      </c>
-      <c r="O11" s="62">
-        <v>1</v>
-      </c>
-      <c r="P11" s="62" t="s">
+      <c r="J11" s="69"/>
+      <c r="K11" s="61">
+        <v>1</v>
+      </c>
+      <c r="L11" s="61">
+        <v>1</v>
+      </c>
+      <c r="M11" s="61">
+        <v>1</v>
+      </c>
+      <c r="N11" s="61">
+        <v>1</v>
+      </c>
+      <c r="O11" s="61">
+        <v>1</v>
+      </c>
+      <c r="P11" s="61" t="s">
         <v>558</v>
       </c>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62" t="s">
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61" t="s">
         <v>214</v>
       </c>
     </row>
@@ -8381,369 +8108,369 @@
       <c r="A12" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="65" t="s">
         <v>561</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="65" t="s">
         <v>561</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="65" t="s">
         <v>560</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="67"/>
-      <c r="R12" s="67"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
     </row>
     <row r="13" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="D13" s="66" t="s">
+      <c r="D13" s="65" t="s">
         <v>411</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="65" t="s">
         <v>412</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="67"/>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="67"/>
-      <c r="R13" s="67"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
     </row>
     <row r="14" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="65" t="s">
         <v>564</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="65" t="s">
         <v>564</v>
       </c>
-      <c r="D14" s="66" t="s">
+      <c r="D14" s="65" t="s">
         <v>564</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="65" t="s">
         <v>412</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="67"/>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="67"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
     </row>
     <row r="15" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="66" t="s">
-        <v>567</v>
-      </c>
-      <c r="C15" s="66" t="s">
-        <v>567</v>
-      </c>
-      <c r="D15" s="66" t="s">
-        <v>568</v>
-      </c>
-      <c r="E15" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>566</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>566</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>566</v>
+      </c>
+      <c r="E15" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="67"/>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="67"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
     </row>
     <row r="16" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="56"/>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62" t="s">
-        <v>569</v>
-      </c>
-      <c r="E16" s="62" t="s">
-        <v>569</v>
-      </c>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62" t="s">
+      <c r="C16" s="61"/>
+      <c r="D16" s="61" t="s">
+        <v>567</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>567</v>
+      </c>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="62"/>
-      <c r="I16" s="70">
-        <v>1</v>
-      </c>
-      <c r="J16" s="70"/>
-      <c r="K16" s="62">
-        <v>1</v>
-      </c>
-      <c r="L16" s="62">
-        <v>1</v>
-      </c>
-      <c r="M16" s="62">
-        <v>1</v>
-      </c>
-      <c r="N16" s="62">
-        <v>1</v>
-      </c>
-      <c r="O16" s="62">
-        <v>1</v>
-      </c>
-      <c r="P16" s="62" t="s">
-        <v>570</v>
-      </c>
-      <c r="Q16" s="62"/>
-      <c r="R16" s="62" t="s">
+      <c r="H16" s="61"/>
+      <c r="I16" s="69">
+        <v>1</v>
+      </c>
+      <c r="J16" s="69"/>
+      <c r="K16" s="61">
+        <v>1</v>
+      </c>
+      <c r="L16" s="61">
+        <v>1</v>
+      </c>
+      <c r="M16" s="61">
+        <v>1</v>
+      </c>
+      <c r="N16" s="61">
+        <v>1</v>
+      </c>
+      <c r="O16" s="61">
+        <v>1</v>
+      </c>
+      <c r="P16" s="61" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q16" s="61"/>
+      <c r="R16" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="56"/>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62" t="s">
-        <v>571</v>
-      </c>
-      <c r="E17" s="62" t="s">
-        <v>571</v>
-      </c>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62" t="s">
+      <c r="C17" s="61"/>
+      <c r="D17" s="61" t="s">
+        <v>569</v>
+      </c>
+      <c r="E17" s="61" t="s">
+        <v>569</v>
+      </c>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="70">
-        <v>1</v>
-      </c>
-      <c r="J17" s="70"/>
-      <c r="K17" s="62">
-        <v>1</v>
-      </c>
-      <c r="L17" s="62">
-        <v>1</v>
-      </c>
-      <c r="M17" s="62">
-        <v>1</v>
-      </c>
-      <c r="N17" s="62">
-        <v>1</v>
-      </c>
-      <c r="O17" s="62">
-        <v>1</v>
-      </c>
-      <c r="P17" s="62" t="s">
-        <v>570</v>
-      </c>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62" t="s">
+      <c r="H17" s="61"/>
+      <c r="I17" s="69">
+        <v>1</v>
+      </c>
+      <c r="J17" s="69"/>
+      <c r="K17" s="61">
+        <v>1</v>
+      </c>
+      <c r="L17" s="61">
+        <v>1</v>
+      </c>
+      <c r="M17" s="61">
+        <v>1</v>
+      </c>
+      <c r="N17" s="61">
+        <v>1</v>
+      </c>
+      <c r="O17" s="61">
+        <v>1</v>
+      </c>
+      <c r="P17" s="61" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="B18" s="66" t="s">
-        <v>573</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>573</v>
-      </c>
-      <c r="D18" s="66" t="s">
-        <v>573</v>
-      </c>
-      <c r="E18" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>571</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>571</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>571</v>
+      </c>
+      <c r="E18" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="67"/>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="67"/>
-      <c r="R18" s="67"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
     </row>
     <row r="19" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="56"/>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62" t="s">
-        <v>574</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>574</v>
-      </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62" t="s">
+      <c r="C19" s="61"/>
+      <c r="D19" s="61" t="s">
+        <v>572</v>
+      </c>
+      <c r="E19" s="61" t="s">
+        <v>572</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="62"/>
-      <c r="I19" s="70">
-        <v>0</v>
-      </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="62">
-        <v>0</v>
-      </c>
-      <c r="L19" s="62">
-        <v>0</v>
-      </c>
-      <c r="M19" s="62">
-        <v>0</v>
-      </c>
-      <c r="N19" s="62">
-        <v>0</v>
-      </c>
-      <c r="O19" s="62">
-        <v>0</v>
-      </c>
-      <c r="P19" s="62" t="s">
-        <v>579</v>
-      </c>
-      <c r="Q19" s="62"/>
-      <c r="R19" s="62" t="s">
+      <c r="H19" s="61"/>
+      <c r="I19" s="69">
+        <v>0</v>
+      </c>
+      <c r="J19" s="69"/>
+      <c r="K19" s="61">
+        <v>0</v>
+      </c>
+      <c r="L19" s="61">
+        <v>0</v>
+      </c>
+      <c r="M19" s="61">
+        <v>0</v>
+      </c>
+      <c r="N19" s="61">
+        <v>0</v>
+      </c>
+      <c r="O19" s="61">
+        <v>0</v>
+      </c>
+      <c r="P19" s="61" t="s">
+        <v>598</v>
+      </c>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="56"/>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62" t="s">
-        <v>575</v>
-      </c>
-      <c r="E20" s="62" t="s">
-        <v>575</v>
-      </c>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62" t="s">
+      <c r="C20" s="61"/>
+      <c r="D20" s="61" t="s">
+        <v>573</v>
+      </c>
+      <c r="E20" s="61" t="s">
+        <v>573</v>
+      </c>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="62"/>
-      <c r="I20" s="70">
-        <v>0</v>
-      </c>
-      <c r="J20" s="70"/>
-      <c r="K20" s="62">
-        <v>0</v>
-      </c>
-      <c r="L20" s="62">
-        <v>0</v>
-      </c>
-      <c r="M20" s="62">
-        <v>0</v>
-      </c>
-      <c r="N20" s="62">
-        <v>0</v>
-      </c>
-      <c r="O20" s="62">
-        <v>0</v>
-      </c>
-      <c r="P20" s="62" t="s">
-        <v>579</v>
-      </c>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62" t="s">
+      <c r="H20" s="61"/>
+      <c r="I20" s="69">
+        <v>0</v>
+      </c>
+      <c r="J20" s="69"/>
+      <c r="K20" s="61">
+        <v>0</v>
+      </c>
+      <c r="L20" s="61">
+        <v>0</v>
+      </c>
+      <c r="M20" s="61">
+        <v>0</v>
+      </c>
+      <c r="N20" s="61">
+        <v>0</v>
+      </c>
+      <c r="O20" s="61">
+        <v>0</v>
+      </c>
+      <c r="P20" s="61" t="s">
+        <v>577</v>
+      </c>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="56"/>
-      <c r="B21" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62" t="s">
+      <c r="B21" s="61" t="s">
+        <v>555</v>
+      </c>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61" t="s">
+        <v>574</v>
+      </c>
+      <c r="E21" s="61" t="s">
+        <v>574</v>
+      </c>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61" t="s">
+        <v>575</v>
+      </c>
+      <c r="H21" s="61"/>
+      <c r="I21" s="69" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="69"/>
+      <c r="K21" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" s="61" t="s">
         <v>576</v>
       </c>
-      <c r="E21" s="62" t="s">
-        <v>576</v>
-      </c>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62" t="s">
-        <v>577</v>
-      </c>
-      <c r="H21" s="62"/>
-      <c r="I21" s="70" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="70"/>
-      <c r="K21" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="M21" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21" s="62" t="b">
-        <v>1</v>
-      </c>
-      <c r="P21" s="62" t="s">
-        <v>578</v>
-      </c>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62" t="s">
+      <c r="Q21" s="61"/>
+      <c r="R21" s="61" t="s">
         <v>214</v>
       </c>
     </row>
@@ -8751,117 +8478,117 @@
       <c r="A22" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="66" t="s">
-        <v>580</v>
-      </c>
-      <c r="C22" s="66" t="s">
-        <v>580</v>
-      </c>
-      <c r="D22" s="66" t="s">
-        <v>580</v>
-      </c>
-      <c r="E22" s="66" t="s">
+      <c r="B22" s="65" t="s">
+        <v>578</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>578</v>
+      </c>
+      <c r="D22" s="65" t="s">
+        <v>578</v>
+      </c>
+      <c r="E22" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="67"/>
-      <c r="M22" s="67"/>
-      <c r="N22" s="67"/>
-      <c r="O22" s="67"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
     </row>
     <row r="23" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="56"/>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62" t="s">
-        <v>581</v>
-      </c>
-      <c r="E23" s="62" t="s">
-        <v>581</v>
-      </c>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62" t="s">
+      <c r="C23" s="61"/>
+      <c r="D23" s="61" t="s">
+        <v>579</v>
+      </c>
+      <c r="E23" s="61" t="s">
+        <v>579</v>
+      </c>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="62"/>
-      <c r="I23" s="70">
-        <v>1</v>
-      </c>
-      <c r="J23" s="70"/>
-      <c r="K23" s="62">
-        <v>1</v>
-      </c>
-      <c r="L23" s="62">
-        <v>1</v>
-      </c>
-      <c r="M23" s="62">
-        <v>1</v>
-      </c>
-      <c r="N23" s="62">
-        <v>1</v>
-      </c>
-      <c r="O23" s="62">
-        <v>1</v>
-      </c>
-      <c r="P23" s="62" t="s">
-        <v>570</v>
-      </c>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62" t="s">
+      <c r="H23" s="61"/>
+      <c r="I23" s="69">
+        <v>1</v>
+      </c>
+      <c r="J23" s="69"/>
+      <c r="K23" s="61">
+        <v>1</v>
+      </c>
+      <c r="L23" s="61">
+        <v>1</v>
+      </c>
+      <c r="M23" s="61">
+        <v>1</v>
+      </c>
+      <c r="N23" s="61">
+        <v>1</v>
+      </c>
+      <c r="O23" s="61">
+        <v>1</v>
+      </c>
+      <c r="P23" s="61" t="s">
+        <v>602</v>
+      </c>
+      <c r="Q23" s="61"/>
+      <c r="R23" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="56"/>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62" t="s">
-        <v>582</v>
-      </c>
-      <c r="E24" s="62" t="s">
-        <v>582</v>
-      </c>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62" t="s">
+      <c r="C24" s="61"/>
+      <c r="D24" s="61" t="s">
+        <v>580</v>
+      </c>
+      <c r="E24" s="61" t="s">
+        <v>580</v>
+      </c>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H24" s="62"/>
-      <c r="I24" s="70">
+      <c r="H24" s="61"/>
+      <c r="I24" s="69">
         <v>30</v>
       </c>
-      <c r="J24" s="70"/>
-      <c r="K24" s="62">
+      <c r="J24" s="69"/>
+      <c r="K24" s="61">
         <v>30</v>
       </c>
-      <c r="L24" s="62">
+      <c r="L24" s="61">
         <v>30</v>
       </c>
-      <c r="M24" s="62">
+      <c r="M24" s="61">
         <v>30</v>
       </c>
-      <c r="N24" s="62">
+      <c r="N24" s="61">
         <v>30</v>
       </c>
-      <c r="O24" s="62">
+      <c r="O24" s="61">
         <v>30</v>
       </c>
-      <c r="P24" s="62" t="s">
-        <v>583</v>
-      </c>
-      <c r="Q24" s="62"/>
-      <c r="R24" s="62" t="s">
+      <c r="P24" s="61" t="s">
+        <v>581</v>
+      </c>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="61" t="s">
         <v>214</v>
       </c>
     </row>
@@ -8869,117 +8596,117 @@
       <c r="A25" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B25" s="66" t="s">
-        <v>584</v>
-      </c>
-      <c r="C25" s="66" t="s">
-        <v>584</v>
-      </c>
-      <c r="D25" s="66" t="s">
-        <v>584</v>
-      </c>
-      <c r="E25" s="66" t="s">
+      <c r="B25" s="65" t="s">
+        <v>582</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>582</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>582</v>
+      </c>
+      <c r="E25" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="67"/>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="67"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="66"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
     </row>
     <row r="26" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="56"/>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62" t="s">
-        <v>599</v>
-      </c>
-      <c r="E26" s="62" t="s">
+      <c r="C26" s="61"/>
+      <c r="D26" s="61" t="s">
+        <v>596</v>
+      </c>
+      <c r="E26" s="61" t="s">
+        <v>583</v>
+      </c>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="H26" s="61"/>
+      <c r="I26" s="69" t="s">
         <v>585</v>
       </c>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62" t="s">
-        <v>207</v>
-      </c>
-      <c r="H26" s="62"/>
-      <c r="I26" s="70" t="s">
-        <v>587</v>
-      </c>
-      <c r="J26" s="70"/>
-      <c r="K26" s="62">
-        <v>1</v>
-      </c>
-      <c r="L26" s="62">
-        <v>1</v>
-      </c>
-      <c r="M26" s="62">
-        <v>1</v>
-      </c>
-      <c r="N26" s="62">
-        <v>1</v>
-      </c>
-      <c r="O26" s="62">
-        <v>1</v>
-      </c>
-      <c r="P26" s="62" t="s">
-        <v>588</v>
-      </c>
-      <c r="Q26" s="62"/>
-      <c r="R26" s="62" t="s">
+      <c r="J26" s="69"/>
+      <c r="K26" s="61">
+        <v>1</v>
+      </c>
+      <c r="L26" s="61">
+        <v>1</v>
+      </c>
+      <c r="M26" s="61">
+        <v>1</v>
+      </c>
+      <c r="N26" s="61">
+        <v>1</v>
+      </c>
+      <c r="O26" s="61">
+        <v>1</v>
+      </c>
+      <c r="P26" s="61" t="s">
+        <v>586</v>
+      </c>
+      <c r="Q26" s="61"/>
+      <c r="R26" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="56"/>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62" t="s">
-        <v>598</v>
-      </c>
-      <c r="E27" s="62" t="s">
-        <v>586</v>
-      </c>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62" t="s">
+      <c r="C27" s="61"/>
+      <c r="D27" s="61" t="s">
+        <v>595</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>584</v>
+      </c>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="62"/>
-      <c r="I27" s="70">
-        <v>1</v>
-      </c>
-      <c r="J27" s="70"/>
-      <c r="K27" s="62">
-        <v>1</v>
-      </c>
-      <c r="L27" s="62">
-        <v>1</v>
-      </c>
-      <c r="M27" s="62">
-        <v>1</v>
-      </c>
-      <c r="N27" s="62">
-        <v>1</v>
-      </c>
-      <c r="O27" s="62">
-        <v>1</v>
-      </c>
-      <c r="P27" s="62" t="s">
-        <v>570</v>
-      </c>
-      <c r="Q27" s="62"/>
-      <c r="R27" s="62" t="s">
+      <c r="H27" s="61"/>
+      <c r="I27" s="69">
+        <v>1</v>
+      </c>
+      <c r="J27" s="69"/>
+      <c r="K27" s="61">
+        <v>1</v>
+      </c>
+      <c r="L27" s="61">
+        <v>1</v>
+      </c>
+      <c r="M27" s="61">
+        <v>1</v>
+      </c>
+      <c r="N27" s="61">
+        <v>1</v>
+      </c>
+      <c r="O27" s="61">
+        <v>1</v>
+      </c>
+      <c r="P27" s="61" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61" t="s">
         <v>214</v>
       </c>
     </row>
@@ -8987,117 +8714,117 @@
       <c r="A28" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B28" s="66" t="s">
-        <v>589</v>
-      </c>
-      <c r="C28" s="66" t="s">
-        <v>589</v>
-      </c>
-      <c r="D28" s="66" t="s">
-        <v>589</v>
-      </c>
-      <c r="E28" s="66" t="s">
+      <c r="B28" s="65" t="s">
+        <v>587</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>587</v>
+      </c>
+      <c r="D28" s="65" t="s">
+        <v>587</v>
+      </c>
+      <c r="E28" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="67"/>
-      <c r="N28" s="67"/>
-      <c r="O28" s="67"/>
-      <c r="P28" s="67"/>
-      <c r="Q28" s="67"/>
-      <c r="R28" s="67"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
     </row>
     <row r="29" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="56"/>
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62" t="s">
-        <v>600</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>585</v>
-      </c>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62" t="s">
+      <c r="C29" s="61"/>
+      <c r="D29" s="61" t="s">
+        <v>597</v>
+      </c>
+      <c r="E29" s="61" t="s">
+        <v>583</v>
+      </c>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="H29" s="62"/>
-      <c r="I29" s="70" t="s">
-        <v>590</v>
-      </c>
-      <c r="J29" s="70"/>
-      <c r="K29" s="62">
-        <v>1</v>
-      </c>
-      <c r="L29" s="62">
-        <v>1</v>
-      </c>
-      <c r="M29" s="62">
-        <v>1</v>
-      </c>
-      <c r="N29" s="62">
-        <v>1</v>
-      </c>
-      <c r="O29" s="62">
-        <v>1</v>
-      </c>
-      <c r="P29" s="62" t="s">
-        <v>591</v>
-      </c>
-      <c r="Q29" s="62"/>
-      <c r="R29" s="62" t="s">
+      <c r="H29" s="61"/>
+      <c r="I29" s="69" t="s">
+        <v>588</v>
+      </c>
+      <c r="J29" s="69"/>
+      <c r="K29" s="61">
+        <v>1</v>
+      </c>
+      <c r="L29" s="61">
+        <v>1</v>
+      </c>
+      <c r="M29" s="61">
+        <v>1</v>
+      </c>
+      <c r="N29" s="61">
+        <v>1</v>
+      </c>
+      <c r="O29" s="61">
+        <v>1</v>
+      </c>
+      <c r="P29" s="61" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="61" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="56"/>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62" t="s">
-        <v>586</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>586</v>
-      </c>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62" t="s">
+      <c r="C30" s="61"/>
+      <c r="D30" s="61" t="s">
+        <v>584</v>
+      </c>
+      <c r="E30" s="61" t="s">
+        <v>584</v>
+      </c>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="62"/>
-      <c r="I30" s="70">
-        <v>1</v>
-      </c>
-      <c r="J30" s="70"/>
-      <c r="K30" s="62">
-        <v>1</v>
-      </c>
-      <c r="L30" s="62">
-        <v>1</v>
-      </c>
-      <c r="M30" s="62">
-        <v>1</v>
-      </c>
-      <c r="N30" s="62">
-        <v>1</v>
-      </c>
-      <c r="O30" s="62">
-        <v>1</v>
-      </c>
-      <c r="P30" s="62" t="s">
-        <v>570</v>
-      </c>
-      <c r="Q30" s="62"/>
-      <c r="R30" s="62" t="s">
+      <c r="H30" s="61"/>
+      <c r="I30" s="69">
+        <v>96</v>
+      </c>
+      <c r="J30" s="69"/>
+      <c r="K30" s="61">
+        <v>1</v>
+      </c>
+      <c r="L30" s="61">
+        <v>1</v>
+      </c>
+      <c r="M30" s="61">
+        <v>1</v>
+      </c>
+      <c r="N30" s="61">
+        <v>1</v>
+      </c>
+      <c r="O30" s="61">
+        <v>1</v>
+      </c>
+      <c r="P30" s="61" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q30" s="61"/>
+      <c r="R30" s="61" t="s">
         <v>214</v>
       </c>
     </row>
@@ -9105,73 +8832,73 @@
       <c r="A31" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B31" s="66" t="s">
-        <v>592</v>
-      </c>
-      <c r="C31" s="66" t="s">
-        <v>592</v>
-      </c>
-      <c r="D31" s="66" t="s">
-        <v>592</v>
-      </c>
-      <c r="E31" s="66" t="s">
+      <c r="B31" s="65" t="s">
+        <v>590</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>590</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>590</v>
+      </c>
+      <c r="E31" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
-      <c r="P31" s="67"/>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="67"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="66"/>
     </row>
     <row r="32" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="56"/>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62" t="s">
-        <v>596</v>
-      </c>
-      <c r="E32" s="62" t="s">
+      <c r="C32" s="61"/>
+      <c r="D32" s="61" t="s">
         <v>593</v>
       </c>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62" t="s">
+      <c r="E32" s="61" t="s">
+        <v>591</v>
+      </c>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61" t="s">
         <v>162</v>
       </c>
-      <c r="H32" s="62"/>
-      <c r="I32" s="70">
-        <v>0</v>
-      </c>
-      <c r="J32" s="70"/>
-      <c r="K32" s="62">
-        <v>0</v>
-      </c>
-      <c r="L32" s="62">
-        <v>0</v>
-      </c>
-      <c r="M32" s="62">
-        <v>0</v>
-      </c>
-      <c r="N32" s="62">
-        <v>0</v>
-      </c>
-      <c r="O32" s="62">
-        <v>0</v>
-      </c>
-      <c r="P32" s="62" t="s">
-        <v>594</v>
-      </c>
-      <c r="Q32" s="62"/>
-      <c r="R32" s="62" t="s">
+      <c r="H32" s="61"/>
+      <c r="I32" s="69">
+        <v>0</v>
+      </c>
+      <c r="J32" s="69"/>
+      <c r="K32" s="61">
+        <v>0</v>
+      </c>
+      <c r="L32" s="61">
+        <v>0</v>
+      </c>
+      <c r="M32" s="61">
+        <v>0</v>
+      </c>
+      <c r="N32" s="61">
+        <v>0</v>
+      </c>
+      <c r="O32" s="61">
+        <v>0</v>
+      </c>
+      <c r="P32" s="61" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="61" t="s">
         <v>214</v>
       </c>
     </row>
@@ -9179,73 +8906,191 @@
       <c r="A33" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="B33" s="66" t="s">
-        <v>595</v>
-      </c>
-      <c r="C33" s="66" t="s">
-        <v>595</v>
-      </c>
-      <c r="D33" s="66" t="s">
-        <v>595</v>
-      </c>
-      <c r="E33" s="66" t="s">
+      <c r="B33" s="65" t="s">
+        <v>592</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>592</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>592</v>
+      </c>
+      <c r="E33" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="67"/>
-      <c r="L33" s="67"/>
-      <c r="M33" s="67"/>
-      <c r="N33" s="67"/>
-      <c r="O33" s="67"/>
-      <c r="P33" s="67"/>
-      <c r="Q33" s="67"/>
-      <c r="R33" s="67"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="66"/>
+      <c r="L33" s="66"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="66"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="66"/>
     </row>
     <row r="34" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="56"/>
-      <c r="B34" s="62" t="s">
+      <c r="B34" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62" t="s">
-        <v>597</v>
-      </c>
-      <c r="E34" s="62" t="s">
-        <v>593</v>
-      </c>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62" t="s">
+      <c r="C34" s="61"/>
+      <c r="D34" s="61" t="s">
+        <v>594</v>
+      </c>
+      <c r="E34" s="61" t="s">
+        <v>591</v>
+      </c>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61" t="s">
         <v>162</v>
       </c>
-      <c r="H34" s="62"/>
-      <c r="I34" s="70">
-        <v>0</v>
-      </c>
-      <c r="J34" s="70"/>
-      <c r="K34" s="62">
-        <v>0</v>
-      </c>
-      <c r="L34" s="62">
-        <v>0</v>
-      </c>
-      <c r="M34" s="62">
-        <v>0</v>
-      </c>
-      <c r="N34" s="62">
-        <v>0</v>
-      </c>
-      <c r="O34" s="62">
-        <v>0</v>
-      </c>
-      <c r="P34" s="62" t="s">
-        <v>594</v>
-      </c>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="62" t="s">
+      <c r="H34" s="61"/>
+      <c r="I34" s="69">
+        <v>0</v>
+      </c>
+      <c r="J34" s="69"/>
+      <c r="K34" s="61">
+        <v>0</v>
+      </c>
+      <c r="L34" s="61">
+        <v>0</v>
+      </c>
+      <c r="M34" s="61">
+        <v>0</v>
+      </c>
+      <c r="N34" s="61">
+        <v>0</v>
+      </c>
+      <c r="O34" s="61">
+        <v>0</v>
+      </c>
+      <c r="P34" s="61" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q34" s="61"/>
+      <c r="R34" s="61" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" s="65" t="s">
+        <v>603</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>603</v>
+      </c>
+      <c r="D35" s="65" t="s">
+        <v>603</v>
+      </c>
+      <c r="E35" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="66"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="66"/>
+    </row>
+    <row r="36" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="56"/>
+      <c r="B36" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61" t="s">
+        <v>608</v>
+      </c>
+      <c r="E36" s="61" t="s">
+        <v>604</v>
+      </c>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" s="61"/>
+      <c r="I36" s="69">
+        <v>0</v>
+      </c>
+      <c r="J36" s="69"/>
+      <c r="K36" s="61">
+        <v>0</v>
+      </c>
+      <c r="L36" s="61">
+        <v>0</v>
+      </c>
+      <c r="M36" s="61">
+        <v>0</v>
+      </c>
+      <c r="N36" s="61">
+        <v>0</v>
+      </c>
+      <c r="O36" s="61">
+        <v>0</v>
+      </c>
+      <c r="P36" s="61" t="s">
+        <v>607</v>
+      </c>
+      <c r="Q36" s="61"/>
+      <c r="R36" s="61" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="56"/>
+      <c r="B37" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61" t="s">
+        <v>605</v>
+      </c>
+      <c r="E37" s="61" t="s">
+        <v>605</v>
+      </c>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="H37" s="61"/>
+      <c r="I37" s="69">
+        <v>0</v>
+      </c>
+      <c r="J37" s="69"/>
+      <c r="K37" s="61">
+        <v>0</v>
+      </c>
+      <c r="L37" s="61">
+        <v>0</v>
+      </c>
+      <c r="M37" s="61">
+        <v>0</v>
+      </c>
+      <c r="N37" s="61">
+        <v>0</v>
+      </c>
+      <c r="O37" s="61">
+        <v>0</v>
+      </c>
+      <c r="P37" s="61" t="s">
+        <v>606</v>
+      </c>
+      <c r="Q37" s="61"/>
+      <c r="R37" s="61" t="s">
         <v>214</v>
       </c>
     </row>
@@ -9254,203 +9099,33 @@
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:A15">
-    <cfRule type="cellIs" dxfId="47" priority="122" operator="equal">
+  <conditionalFormatting sqref="A9:A34">
+    <cfRule type="cellIs" dxfId="49" priority="124" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A15">
-    <cfRule type="cellIs" dxfId="46" priority="121" operator="equal">
+  <conditionalFormatting sqref="A9:A34">
+    <cfRule type="cellIs" dxfId="48" priority="123" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="45" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="117" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="44" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="118" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A21">
-    <cfRule type="cellIs" dxfId="43" priority="29" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
+  <conditionalFormatting sqref="A35:A37">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="41" priority="37" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="cellIs" dxfId="40" priority="23" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A21">
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="A35:A37">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15305,7 +14980,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="28" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Added correct output for btapresults
</commit_message>
<xml_diff>
--- a/projects/NECB_QA_QC.xlsx
+++ b/projects/NECB_QA_QC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5670" windowWidth="20370" windowHeight="4845" tabRatio="469" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="5670" windowWidth="19440" windowHeight="4845" tabRatio="469" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="482">
   <si>
     <t>type</t>
   </si>
@@ -822,13 +822,667 @@
     <t>1.21.15-nrcan</t>
   </si>
   <si>
-    <t>["FullServiceRestaurant","HighriseApartment","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
-  </si>
-  <si>
     <t>../../OpenStudio-measures/NRCAN_working_measures</t>
   </si>
   <si>
     <t>['CAN_AB_Calgary.718770_CWEC.epw']</t>
+  </si>
+  <si>
+    <t>btapresults.econ_district_cooling_total_cost_intensity_dollars_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.econ_district_heating_total_cost_intensity_dollars_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.econ_electricity_total_cost_intensity_dollars_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.econ_natural_gas_total_cost_intensity_dollars_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.econ_total_utility_cost</t>
+  </si>
+  <si>
+    <t>btapresults.econ_virtual_rate_combined_dollars_per_gj</t>
+  </si>
+  <si>
+    <t>btapresults.econ_virtual_rate_elect_dollars_per_gj</t>
+  </si>
+  <si>
+    <t>btapresults.econ_virtual_rate_gas_dollars_per_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_cooling_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_exterior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_exterior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_fans_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_generators_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_heat_recovery_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_heat_rejection_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_heating_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_humidification_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_interior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_interior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_pumps_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_refrigeration_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_total_end_uses_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_additional_fuel_water_systems_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_cooling_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_exterior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_exterior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_fans_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_generators_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_heat_recovery_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_heat_rejection_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_heating_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_humidification_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_interior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_interior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_pumps_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_refrigeration_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_total_end_uses_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_cooling_water_systems_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_cooling_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_exterior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_exterior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_fans_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_generators_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_heat_recovery_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_heat_rejection_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_heating_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_humidification_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_interior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_interior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_pumps_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_refrigeration_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_total_end_uses_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_district_heating_water_systems_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_cooling_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_exterior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_exterior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_fans_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_generators_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_heat_recovery_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_heat_rejection_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_heating_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_humidification_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_interior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_interior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_pumps_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_refrigeration_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_total_end_uses_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_electricity_water_systems_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_cooling_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_exterior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_exterior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_fans_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_generators_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_heat_recovery_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_heat_rejection_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_heating_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_humidification_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_interior_equipment_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_interior_lighting_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_pumps_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_refrigeration_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_total_end_uses_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_natural_gas_water_systems_gj</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_cooling_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_exterior_equipment_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_exterior_lighting_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_fans_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_generators_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_heat_recovery_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_heat_rejection_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_heating_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_humidification_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_interior_equipment_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_interior_lighting_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_pumps_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_refrigeration_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_total_end_uses_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.end_use_water_water_systems_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_building_volume_m_3</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_conditioned_floor_area_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_exterior_surface_area_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_fdwr_ratio</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_outdoor_doors_average_conductance_w_per_m_2_k</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_outdoor_floors_average_conductance_w_per_m_2_k</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_outdoor_overhead_doors_average_conductance_w_per_m_2_k</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_outdoor_roofs_average_conductance_w_per_m_2_k</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_outdoor_walls_average_conductance_w_per_m_2_k</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_outdoor_windows_average_conductance_w_per_m_2_k</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_skylights_average_conductance_w_per_m_2_k</t>
+  </si>
+  <si>
+    <t>btapresults.envelope_srr_ratio</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_cooling_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_exterior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_exterior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_fans_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_generators_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_heat_recovery_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_heat_rejection_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_heating_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_humidification_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_interior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_interior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_pumps_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_refrigeration_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_total_end_uses_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_additional_fuel_water_systems_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_cooling_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_exterior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_exterior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_fans_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_generators_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_heat_recovery_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_heat_rejection_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_heating_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_humidification_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_interior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_interior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_pumps_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_refrigeration_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_total_end_uses_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_cooling_water_systems_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_cooling_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_exterior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_exterior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_fans_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_generators_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_heat_recovery_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_heat_rejection_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_heating_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_humidification_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_interior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_interior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_pumps_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_refrigeration_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_total_end_uses_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_district_heating_water_systems_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_cooling_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_exterior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_exterior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_fans_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_generators_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_heat_recovery_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_heat_rejection_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_heating_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_humidification_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_interior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_interior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_pumps_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_refrigeration_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_total_end_uses_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_electricity_water_systems_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_cooling_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_exterior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_exterior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_fans_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_generators_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_heat_recovery_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_heat_rejection_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_heating_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_humidification_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_interior_equipment_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_interior_lighting_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_pumps_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_refrigeration_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_total_end_uses_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_natural_gas_water_systems_gj_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_cooling_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_exterior_equipment_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_exterior_lighting_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_fans_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_generators_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_heat_recovery_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_heat_rejection_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_heating_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_humidification_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_interior_equipment_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_interior_lighting_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_pumps_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_refrigeration_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_total_end_uses_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.eui_water_water_systems_m_3_per_m_2</t>
+  </si>
+  <si>
+    <t>btapresults.geo_city</t>
+  </si>
+  <si>
+    <t>btapresults.geo_coolingdegreedays_dd</t>
+  </si>
+  <si>
+    <t>btapresults.geo_country</t>
+  </si>
+  <si>
+    <t>btapresults.geo_datasource</t>
+  </si>
+  <si>
+    <t>btapresults.geo_heatingdegreedays_dd</t>
+  </si>
+  <si>
+    <t>btapresults.geo_latitude_deg</t>
+  </si>
+  <si>
+    <t>btapresults.geo_longitude_deg</t>
+  </si>
+  <si>
+    <t>btapresults.geo_necb_climate_zone</t>
+  </si>
+  <si>
+    <t>btapresults.geo_province</t>
+  </si>
+  <si>
+    <t>btapresults.geo_wmonumber</t>
+  </si>
+  <si>
+    <t>btapresults.peak_electricy_power_watts</t>
+  </si>
+  <si>
+    <t>btapresults.peak_natural_gas_watts</t>
+  </si>
+  <si>
+    <t>btapresults.qaqc_unmet_hours_cooling_hours</t>
+  </si>
+  <si>
+    <t>btapresults.qaqc_unmet_hours_heating_hours</t>
+  </si>
+  <si>
+    <t>btapresults.source</t>
+  </si>
+  <si>
+    <t>btapresults.applicable</t>
+  </si>
+  <si>
+    <t>["FullServiceRestaurant","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
+  </si>
+  <si>
+    <t>view_model.view_model_html_zip</t>
+  </si>
+  <si>
+    <t>btapresults.model_osm_zip</t>
   </si>
 </sst>
 </file>
@@ -5839,7 +6493,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="29" t="s">
@@ -6130,7 +6784,7 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -6344,7 +6998,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>261</v>
+        <v>479</v>
       </c>
       <c r="Q5" s="54"/>
       <c r="R5" s="54" t="s">
@@ -6476,7 +7130,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q8" s="54"/>
       <c r="R8" s="54" t="s">
@@ -6679,11 +7333,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="3" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D230" sqref="D230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6795,6 +7449,3712 @@
       </c>
       <c r="M3" s="38" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="G5" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="G7" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="G8" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="G9" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="G10" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="G11" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="G12" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="G13" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="G14" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="G16" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="G17" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="G18" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="G19" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="G20" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="G21" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="G22" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="G23" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="G24" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="G25" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="G26" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="G27" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="G28" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="G29" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="G30" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="G31" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="G32" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="G33" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="G34" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="G35" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="G36" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="G37" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="G38" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="G39" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="G40" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="G41" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="G42" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="G43" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="G44" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="G45" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="G46" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="G47" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="G48" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="G49" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="G50" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="G51" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="G52" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="D53" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="G53" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="G54" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="D55" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="G55" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="G56" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="D57" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="G57" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="G58" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="G59" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="G60" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="G61" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="G62" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="G63" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H63" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="G64" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="G65" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="G66" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G67" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="G68" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="G69" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I69" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="G70" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I70" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="G71" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H71" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="G72" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H72" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I72" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="D73" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="G73" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H73" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I73" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="G74" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="G75" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H75" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I75" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="G76" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H76" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="G77" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="G78" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I78" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="D79" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="G79" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H79" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I79" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="D80" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="G80" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H80" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G81" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H81" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="D82" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="G82" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H82" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="D83" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="G83" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="G84" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H84" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="D85" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="G85" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="G86" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I86" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="G87" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H87" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I87" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="D88" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="G88" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H88" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I88" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="D89" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G89" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I89" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="D90" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G90" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I90" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="D91" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="G91" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H91" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I91" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="G92" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H92" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I92" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="D93" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="G93" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H93" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I93" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="G94" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H94" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I94" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="D95" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="G95" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G96" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I96" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="29" t="s">
+        <v>356</v>
+      </c>
+      <c r="D97" s="29" t="s">
+        <v>356</v>
+      </c>
+      <c r="G97" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H97" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I97" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="G98" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I98" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="G99" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H99" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="D100" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G100" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H100" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I100" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="D101" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="G101" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H101" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I101" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="D102" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="G102" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H102" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="D103" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="G103" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H103" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I103" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="G104" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H104" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I104" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="D105" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="G105" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H105" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I105" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="D106" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="G106" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H106" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I106" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="29" t="s">
+        <v>366</v>
+      </c>
+      <c r="D107" s="29" t="s">
+        <v>366</v>
+      </c>
+      <c r="G107" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H107" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I107" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="D108" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="G108" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H108" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I108" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="29" t="s">
+        <v>368</v>
+      </c>
+      <c r="D109" s="29" t="s">
+        <v>368</v>
+      </c>
+      <c r="G109" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H109" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I109" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D110" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="G110" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H110" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I110" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="D111" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="G111" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H111" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I111" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="D112" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="G112" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H112" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I112" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="D113" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="G113" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H113" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I113" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="29" t="s">
+        <v>373</v>
+      </c>
+      <c r="D114" s="29" t="s">
+        <v>373</v>
+      </c>
+      <c r="G114" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H114" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I114" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="D115" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="G115" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I115" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="D116" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="G116" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H116" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I116" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="29" t="s">
+        <v>376</v>
+      </c>
+      <c r="D117" s="29" t="s">
+        <v>376</v>
+      </c>
+      <c r="G117" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H117" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I117" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D118" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="G118" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H118" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I118" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="D119" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="G119" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H119" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I119" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="D120" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="G120" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I120" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="D121" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="G121" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H121" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="29" t="s">
+        <v>381</v>
+      </c>
+      <c r="D122" s="29" t="s">
+        <v>381</v>
+      </c>
+      <c r="G122" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H122" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I122" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="29" t="s">
+        <v>382</v>
+      </c>
+      <c r="D123" s="29" t="s">
+        <v>382</v>
+      </c>
+      <c r="G123" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H123" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I123" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="D124" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="G124" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H124" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="D125" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="G125" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H125" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="D126" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="G126" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H126" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I126" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="D127" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="G127" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H127" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I127" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="29" t="s">
+        <v>387</v>
+      </c>
+      <c r="D128" s="29" t="s">
+        <v>387</v>
+      </c>
+      <c r="G128" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H128" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I128" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="D129" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="G129" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H129" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I129" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="D130" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="G130" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H130" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I130" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="D131" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="G131" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H131" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I131" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="D132" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="G132" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H132" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I132" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="D133" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="G133" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H133" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I133" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="D134" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="G134" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H134" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I134" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="D135" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="G135" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H135" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I135" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="29" t="s">
+        <v>395</v>
+      </c>
+      <c r="D136" s="29" t="s">
+        <v>395</v>
+      </c>
+      <c r="G136" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H136" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I136" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="D137" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="G137" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H137" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I137" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="29" t="s">
+        <v>397</v>
+      </c>
+      <c r="D138" s="29" t="s">
+        <v>397</v>
+      </c>
+      <c r="G138" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H138" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I138" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="D139" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="G139" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H139" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I139" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="D140" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="G140" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H140" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I140" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="D141" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="G141" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H141" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I141" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="D142" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="G142" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H142" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I142" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="D143" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="G143" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H143" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I143" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="D144" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="G144" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H144" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I144" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="D145" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="G145" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H145" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I145" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="D146" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="G146" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H146" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I146" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="D147" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="G147" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H147" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I147" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="D148" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="G148" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H148" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I148" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D149" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="G149" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H149" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I149" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="D150" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="G150" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H150" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I150" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="29" t="s">
+        <v>410</v>
+      </c>
+      <c r="D151" s="29" t="s">
+        <v>410</v>
+      </c>
+      <c r="G151" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H151" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I151" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="29" t="s">
+        <v>411</v>
+      </c>
+      <c r="D152" s="29" t="s">
+        <v>411</v>
+      </c>
+      <c r="G152" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H152" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I152" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="D153" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="G153" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H153" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I153" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="D154" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="G154" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H154" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I154" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="D155" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="G155" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H155" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I155" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="D156" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="G156" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H156" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I156" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="D157" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="G157" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H157" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I157" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="D158" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="G158" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H158" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I158" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="D159" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="G159" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H159" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I159" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="29" t="s">
+        <v>419</v>
+      </c>
+      <c r="D160" s="29" t="s">
+        <v>419</v>
+      </c>
+      <c r="G160" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H160" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I160" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" s="29" t="s">
+        <v>420</v>
+      </c>
+      <c r="D161" s="29" t="s">
+        <v>420</v>
+      </c>
+      <c r="G161" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H161" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I161" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="D162" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="G162" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H162" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I162" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" s="29" t="s">
+        <v>422</v>
+      </c>
+      <c r="D163" s="29" t="s">
+        <v>422</v>
+      </c>
+      <c r="G163" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H163" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I163" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="D164" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="G164" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H164" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I164" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="D165" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="G165" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H165" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I165" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="D166" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="G166" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H166" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I166" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="D167" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="G167" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H167" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I167" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="D168" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="G168" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H168" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I168" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="D169" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="G169" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H169" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I169" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="D170" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="G170" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H170" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I170" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A171" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="D171" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="G171" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H171" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I171" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="D172" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="G172" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H172" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I172" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="D173" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="G173" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H173" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I173" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="D174" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="G174" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H174" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I174" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="D175" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="G175" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H175" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I175" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="D176" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="G176" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H176" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I176" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="D177" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="G177" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H177" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I177" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="D178" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="G178" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H178" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I178" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="D179" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="G179" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H179" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I179" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="D180" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="G180" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H180" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I180" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="D181" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="G181" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H181" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I181" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="D182" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="G182" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H182" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I182" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="D183" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="G183" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H183" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I183" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="D184" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="G184" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H184" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I184" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="D185" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="G185" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H185" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I185" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="29" t="s">
+        <v>445</v>
+      </c>
+      <c r="D186" s="29" t="s">
+        <v>445</v>
+      </c>
+      <c r="G186" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H186" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I186" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="D187" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="G187" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H187" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I187" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="D188" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="G188" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H188" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I188" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="D189" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="G189" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H189" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I189" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190" s="29" t="s">
+        <v>449</v>
+      </c>
+      <c r="D190" s="29" t="s">
+        <v>449</v>
+      </c>
+      <c r="G190" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H190" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I190" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191" s="29" t="s">
+        <v>450</v>
+      </c>
+      <c r="D191" s="29" t="s">
+        <v>450</v>
+      </c>
+      <c r="G191" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H191" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I191" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="D192" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="G192" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H192" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I192" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="D193" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="G193" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H193" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I193" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="D194" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="G194" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H194" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I194" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="D195" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="G195" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H195" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I195" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="D196" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="G196" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H196" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I196" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="D197" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="G197" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H197" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I197" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="D198" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="G198" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H198" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I198" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="D199" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="G199" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H199" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I199" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="D200" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="G200" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H200" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I200" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="D201" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="G201" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H201" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I201" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="D202" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="G202" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H202" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I202" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="D203" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="G203" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H203" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I203" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="D204" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="G204" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H204" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I204" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="D205" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="G205" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H205" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I205" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="D206" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="G206" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H206" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I206" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="D207" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="G207" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H207" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I207" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="D208" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="G208" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H208" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I208" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="D209" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="G209" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H209" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I209" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A210" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="D210" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="G210" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H210" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I210" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A211" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="D211" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="G211" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H211" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I211" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A212" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="D212" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="G212" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H212" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I212" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A213" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="D213" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="G213" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H213" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I213" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A214" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="D214" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="G214" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H214" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I214" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A215" s="29" t="s">
+        <v>474</v>
+      </c>
+      <c r="D215" s="29" t="s">
+        <v>474</v>
+      </c>
+      <c r="G215" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H215" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I215" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="D216" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="G216" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H216" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I216" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A217" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="D217" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="G217" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H217" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I217" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="D218" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="G218" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H218" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I218" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A219" s="29" t="s">
+        <v>481</v>
+      </c>
+      <c r="D219" s="29" t="s">
+        <v>481</v>
+      </c>
+      <c r="G219" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H219" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I219" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A220" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="D220" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="G220" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H220" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I220" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A221" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="D221" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="G221" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H221" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I221" s="29" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for btaps_results json file for Padmassun.
</commit_message>
<xml_diff>
--- a/projects/NECB_QA_QC.xlsx
+++ b/projects/NECB_QA_QC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5670" windowWidth="19440" windowHeight="4845" tabRatio="469" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="5790" windowWidth="19440" windowHeight="4725" tabRatio="469" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="483">
   <si>
     <t>type</t>
   </si>
@@ -789,12 +789,6 @@
     <t>write_your_analysis_name_here</t>
   </si>
   <si>
-    <t>Inventory</t>
-  </si>
-  <si>
-    <t>generic_qaqc</t>
-  </si>
-  <si>
     <t>argument</t>
   </si>
   <si>
@@ -807,9 +801,6 @@
     <t>["90.1-2010"]</t>
   </si>
   <si>
-    <t>GenericQAQC</t>
-  </si>
-  <si>
     <t>ViewModel</t>
   </si>
   <si>
@@ -825,9 +816,6 @@
     <t>../../OpenStudio-measures/NRCAN_working_measures</t>
   </si>
   <si>
-    <t>['CAN_AB_Calgary.718770_CWEC.epw']</t>
-  </si>
-  <si>
     <t>btapresults.econ_district_cooling_total_cost_intensity_dollars_per_m_2</t>
   </si>
   <si>
@@ -1476,13 +1464,28 @@
     <t>btapresults.applicable</t>
   </si>
   <si>
+    <t>view_model.view_model_html_zip</t>
+  </si>
+  <si>
+    <t>btapresults.model_osm_zip</t>
+  </si>
+  <si>
+    <t>Working Weather Files</t>
+  </si>
+  <si>
+    <t>["CAN_ON_Simcoe.715270_CWEC.epw","CAN_PQ_Nitchequon.CAN270_CWEC.epw","CAN_ON_Kingston.716200_CWEC.epw","CAN_NS_Truro.713980_CWEC.epw","CAN_ON_Muskoka.716300_CWEC.epw","CAN_PQ_Montreal.Jean.Brebeuf.716278_CWEC.epw","CAN_NF_Battle.Harbour.718170_CWEC.epw","CAN_PQ_Montreal.Mirabel.716278_CWEC.epw","CAN_PQ_Grindstone.Island_CWEC.epw"]</t>
+  </si>
+  <si>
+    <t>Broken Weather Files</t>
+  </si>
+  <si>
+    <t>['CAN_AB_Calgary.718770_CWEC.epw','CAN_AB_Edmonton.711230_CWEC.epw','CAN_AB_Fort.McMurray.719320_CWEC.epw','CAN_AB_Grande.Prairie.719400_CWEC.epw','CAN_AB_Lethbridge.712430_CWEC.epw','CAN_AB_Medicine.Hat.718720_CWEC.epw','CAN_BC_Abbotsford.711080_CWEC.epw','CAN_BC_Comox.718930_CWEC.epw','CAN_BC_Cranbrook.718800_CWEC.epw','CAN_BC_Fort.St.John.719430_CWEC.epw','CAN_BC_Kamloops.718870_CWEC.epw','CAN_BC_Port.Hardy.711090_CWEC.epw','CAN_BC_Prince.George.718960_CWEC.epw','CAN_BC_Prince.Rupert.718980_CWEC.epw','CAN_BC_Sandspit.711010_CWEC.epw','CAN_BC_Smithers.719500_CWEC.epw','CAN_BC_Summerland.717680_CWEC.epw','CAN_BC_Vancouver.718920_CWEC.epw','CAN_BC_Victoria.717990_CWEC.epw','CAN_MB_Brandon.711400_CWEC.epw','CAN_MB_Churchill.719130_CWEC.epw','CAN_MB_The.Pas.718670_CWEC.epw','CAN_MB_Winnipeg.718520_CWEC.epw','CAN_NB_Fredericton.717000_CWEC.epw','CAN_NB_Miramichi.717440_CWEC.epw','CAN_NB_Saint.John.716090_CWEC.epw','CAN_NF_Gander.718030_CWEC.epw','CAN_NF_Goose.718160_CWEC.epw','CAN_NF_St.Johns.718010_CWEC.epw','CAN_NF_Stephenville.718150_CWEC.epw','CAN_NS_Greenwood.713970_CWEC.epw','CAN_NS_Sable.Island.716000_CWEC.epw','CAN_NS_Shearwater.716010_CWEC.epw','CAN_NS_Sydney.717070_CWEC.epw','CAN_NT_Inuvik.719570_CWEC.epw','CAN_NU_Resolute.719240_CWEC.epw','CAN_ON_London.716230_CWEC.epw','CAN_ON_Mount.Forest.716310_CWEC.epw','CAN_ON_North.Bay.717310_CWEC.epw','CAN_ON_Ottawa.716280_CWEC.epw','CAN_ON_Sault.Ste.Marie.712600_CWEC.epw','CAN_ON_Thunder.Bay.717490_CWEC.epw','CAN_ON_Timmins.717390_CWEC.epw','CAN_ON_Toronto.716240_CWEC.epw','CAN_ON_Trenton.716210_CWEC.epw','CAN_ON_Windsor.715380_CWEC.epw','CAN_PE_Charlottetown.717060_CWEC.epw','CAN_PQ_Bagotville.717270_CWEC.epw','CAN_PQ_Baie.Comeau.711870_CWEC.epw','CAN_PQ_Kuujjuarapik.719050_CWEC.epw','CAN_PQ_Kuujuaq.719060_CWEC.epw','CAN_PQ_La.Grande.Riviere.718270_CWEC.epw','CAN_PQ_Lake.Eon.714210_CWEC.epw','CAN_PQ_Mont.Joli.717180_CWEC.epw','CAN_PQ_Montreal.Intl.AP.716270_CWEC.epw','CAN_PQ_Quebec.717140_CWEC.epw','CAN_PQ_Riviere.du.Loup.717150_CWEC.epw','CAN_PQ_Roberval.717280_CWEC.epw','CAN_PQ_Schefferville.718280_CWEC.epw','CAN_PQ_Sept-Iles.718110_CWEC.epw','CAN_PQ_Sherbrooke.716100_CWEC.epw','CAN_PQ_St.Hubert.713710_CWEC.epw','CAN_PQ_Ste.Agathe.des.Monts.717200_CWEC.epw','CAN_PQ_Val.d.Or.717250_CWEC.epw','CAN_SK_Estevan.718620_CWEC.epw','CAN_SK_North.Battleford.718760_CWEC.epw','CAN_SK_Regina.718630_CWEC.epw','CAN_SK_Saskatoon.718660_CWEC.epw','CAN_SK_Swift.Current.718700_CWEC.epw','CAN_YT_Whitehorse.719640_CWEC.epw']</t>
+  </si>
+  <si>
     <t>["FullServiceRestaurant","LargeHotel","LargeOffice","MediumOffice","MidriseApartment","Outpatient","PrimarySchool","QuickServiceRestaurant","RetailStandalone","SecondarySchool","SmallHotel","SmallOffice","RetailStripmall","Warehouse"]</t>
   </si>
   <si>
-    <t>view_model.view_model_html_zip</t>
-  </si>
-  <si>
-    <t>btapresults.model_osm_zip</t>
+    <t>btapresults.btap_results_json_zip</t>
   </si>
 </sst>
 </file>
@@ -3952,7 +3955,7 @@
     <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4056,7 +4059,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4066,7 +4068,6 @@
     <xf numFmtId="0" fontId="29" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6318,7 +6319,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6376,7 +6377,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>157</v>
@@ -6387,7 +6388,7 @@
         <v>75</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>77</v>
@@ -6436,7 +6437,7 @@
         <v>66</v>
       </c>
       <c r="B9" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="30"/>
@@ -6493,7 +6494,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="29" t="s">
@@ -6781,10 +6782,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -6839,14 +6840,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="63" t="s">
+      <c r="U1" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -6963,355 +6964,295 @@
     </row>
     <row r="5" spans="1:26" s="46" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54" t="s">
+      <c r="C5" s="53"/>
+      <c r="D5" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="53" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54" t="s">
+      <c r="F5" s="53"/>
+      <c r="G5" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="53"/>
+      <c r="I5" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="55"/>
-      <c r="K5" s="56">
-        <v>1</v>
-      </c>
-      <c r="L5" s="56">
-        <v>1</v>
-      </c>
-      <c r="M5" s="56">
-        <v>1</v>
-      </c>
-      <c r="N5" s="56">
-        <v>1</v>
-      </c>
-      <c r="O5" s="56">
+      <c r="J5" s="54"/>
+      <c r="K5" s="55">
+        <v>1</v>
+      </c>
+      <c r="L5" s="55">
+        <v>1</v>
+      </c>
+      <c r="M5" s="55">
+        <v>1</v>
+      </c>
+      <c r="N5" s="55">
+        <v>1</v>
+      </c>
+      <c r="O5" s="55">
         <v>1</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>479</v>
-      </c>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="46" customFormat="1" ht="14.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54" t="s">
+      <c r="C6" s="53"/>
+      <c r="D6" s="53" t="s">
         <v>190</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54" t="s">
+      <c r="F6" s="53"/>
+      <c r="G6" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54" t="s">
+      <c r="H6" s="53"/>
+      <c r="I6" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="56">
-        <v>1</v>
-      </c>
-      <c r="L6" s="56">
-        <v>1</v>
-      </c>
-      <c r="M6" s="56">
-        <v>1</v>
-      </c>
-      <c r="N6" s="56">
-        <v>1</v>
-      </c>
-      <c r="O6" s="56">
-        <v>1</v>
-      </c>
-      <c r="P6" s="54" t="s">
+      <c r="J6" s="53"/>
+      <c r="K6" s="55">
+        <v>1</v>
+      </c>
+      <c r="L6" s="55">
+        <v>1</v>
+      </c>
+      <c r="M6" s="55">
+        <v>1</v>
+      </c>
+      <c r="N6" s="55">
+        <v>1</v>
+      </c>
+      <c r="O6" s="55">
+        <v>1</v>
+      </c>
+      <c r="P6" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54" t="s">
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="46" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54" t="s">
+      <c r="C7" s="53"/>
+      <c r="D7" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="53" t="s">
         <v>191</v>
       </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54" t="s">
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="H7" s="54"/>
-      <c r="I7" s="57" t="s">
+      <c r="H7" s="53"/>
+      <c r="I7" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="J7" s="54"/>
-      <c r="K7" s="56">
-        <v>1</v>
-      </c>
-      <c r="L7" s="56">
-        <v>1</v>
-      </c>
-      <c r="M7" s="56">
-        <v>1</v>
-      </c>
-      <c r="N7" s="56">
-        <v>1</v>
-      </c>
-      <c r="O7" s="56">
-        <v>1</v>
-      </c>
-      <c r="P7" s="57" t="s">
+      <c r="J7" s="53"/>
+      <c r="K7" s="55">
+        <v>1</v>
+      </c>
+      <c r="L7" s="55">
+        <v>1</v>
+      </c>
+      <c r="M7" s="55">
+        <v>1</v>
+      </c>
+      <c r="N7" s="55">
+        <v>1</v>
+      </c>
+      <c r="O7" s="55">
+        <v>1</v>
+      </c>
+      <c r="P7" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54" t="s">
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="46" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54" t="s">
+      <c r="F8" s="53"/>
+      <c r="G8" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="H8" s="54"/>
-      <c r="I8" s="57" t="s">
+      <c r="H8" s="53"/>
+      <c r="I8" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="56">
-        <v>1</v>
-      </c>
-      <c r="L8" s="56">
-        <v>1</v>
-      </c>
-      <c r="M8" s="56">
-        <v>1</v>
-      </c>
-      <c r="N8" s="56">
-        <v>1</v>
-      </c>
-      <c r="O8" s="56">
+      <c r="J8" s="53"/>
+      <c r="K8" s="55">
+        <v>1</v>
+      </c>
+      <c r="L8" s="55">
+        <v>1</v>
+      </c>
+      <c r="M8" s="55">
+        <v>1</v>
+      </c>
+      <c r="N8" s="55">
+        <v>1</v>
+      </c>
+      <c r="O8" s="55">
         <v>1</v>
       </c>
       <c r="P8" s="43" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="58" t="s">
+    <row r="9" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="53" t="s">
         <v>250</v>
       </c>
-      <c r="C9" s="58" t="s">
-        <v>250</v>
-      </c>
-      <c r="D9" s="58" t="s">
-        <v>250</v>
-      </c>
-      <c r="E9" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="60"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="60" t="s">
+        <v>252</v>
+      </c>
       <c r="J9" s="60"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="59"/>
+      <c r="K9" s="53">
+        <v>1</v>
+      </c>
+      <c r="L9" s="53">
+        <v>1</v>
+      </c>
+      <c r="M9" s="53">
+        <v>1</v>
+      </c>
+      <c r="N9" s="53">
+        <v>1</v>
+      </c>
+      <c r="O9" s="53">
+        <v>1</v>
+      </c>
+      <c r="P9" s="53" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="53" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="10" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B10" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="C10" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="D10" s="58" t="s">
-        <v>256</v>
-      </c>
-      <c r="E10" s="58" t="s">
+      <c r="B10" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+    </row>
+    <row r="11" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="E11" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-    </row>
-    <row r="11" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="54" t="s">
-        <v>252</v>
-      </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54" t="s">
-        <v>253</v>
-      </c>
-      <c r="E11" s="54" t="s">
-        <v>197</v>
-      </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54" t="s">
-        <v>188</v>
-      </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="62" t="s">
-        <v>254</v>
-      </c>
-      <c r="J11" s="62"/>
-      <c r="K11" s="54">
-        <v>1</v>
-      </c>
-      <c r="L11" s="54">
-        <v>1</v>
-      </c>
-      <c r="M11" s="54">
-        <v>1</v>
-      </c>
-      <c r="N11" s="54">
-        <v>1</v>
-      </c>
-      <c r="O11" s="54">
-        <v>1</v>
-      </c>
-      <c r="P11" s="54" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="54" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="58" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" s="58" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="58" t="s">
-        <v>257</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="59"/>
-    </row>
-    <row r="13" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B13" s="58" t="s">
-        <v>214</v>
-      </c>
-      <c r="C13" s="58" t="s">
-        <v>214</v>
-      </c>
-      <c r="D13" s="58" t="s">
-        <v>214</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>215</v>
-      </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="59"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA7"/>
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:A13">
+  <conditionalFormatting sqref="A9:A11">
     <cfRule type="cellIs" dxfId="3" priority="126" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A13">
+  <conditionalFormatting sqref="A9:A11">
     <cfRule type="cellIs" dxfId="2" priority="125" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -7333,11 +7274,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M221"/>
+  <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D230" sqref="D230"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I223" sqref="I223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7453,10 +7394,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G4" s="29" t="b">
         <v>1</v>
@@ -7470,10 +7411,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G5" s="29" t="b">
         <v>1</v>
@@ -7487,10 +7428,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G6" s="29" t="b">
         <v>1</v>
@@ -7504,10 +7445,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G7" s="29" t="b">
         <v>1</v>
@@ -7521,10 +7462,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G8" s="29" t="b">
         <v>1</v>
@@ -7538,10 +7479,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G9" s="29" t="b">
         <v>1</v>
@@ -7555,10 +7496,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="G10" s="29" t="b">
         <v>1</v>
@@ -7572,10 +7513,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G11" s="29" t="b">
         <v>1</v>
@@ -7589,10 +7530,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="G12" s="29" t="b">
         <v>1</v>
@@ -7606,10 +7547,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G13" s="29" t="b">
         <v>1</v>
@@ -7623,10 +7564,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G14" s="29" t="b">
         <v>1</v>
@@ -7640,10 +7581,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G15" s="29" t="b">
         <v>1</v>
@@ -7657,10 +7598,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G16" s="29" t="b">
         <v>1</v>
@@ -7674,10 +7615,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G17" s="29" t="b">
         <v>1</v>
@@ -7691,10 +7632,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G18" s="29" t="b">
         <v>1</v>
@@ -7708,10 +7649,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G19" s="29" t="b">
         <v>1</v>
@@ -7725,10 +7666,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G20" s="29" t="b">
         <v>1</v>
@@ -7742,10 +7683,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G21" s="29" t="b">
         <v>1</v>
@@ -7759,10 +7700,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="G22" s="29" t="b">
         <v>1</v>
@@ -7776,10 +7717,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G23" s="29" t="b">
         <v>1</v>
@@ -7793,10 +7734,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G24" s="29" t="b">
         <v>1</v>
@@ -7810,10 +7751,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G25" s="29" t="b">
         <v>1</v>
@@ -7827,10 +7768,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G26" s="29" t="b">
         <v>1</v>
@@ -7844,10 +7785,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="G27" s="29" t="b">
         <v>1</v>
@@ -7861,10 +7802,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G28" s="29" t="b">
         <v>1</v>
@@ -7878,10 +7819,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G29" s="29" t="b">
         <v>1</v>
@@ -7895,10 +7836,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G30" s="29" t="b">
         <v>1</v>
@@ -7912,10 +7853,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G31" s="29" t="b">
         <v>1</v>
@@ -7929,10 +7870,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G32" s="29" t="b">
         <v>1</v>
@@ -7946,10 +7887,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G33" s="29" t="b">
         <v>1</v>
@@ -7963,10 +7904,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G34" s="29" t="b">
         <v>1</v>
@@ -7980,10 +7921,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G35" s="29" t="b">
         <v>1</v>
@@ -7997,10 +7938,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G36" s="29" t="b">
         <v>1</v>
@@ -8014,10 +7955,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G37" s="29" t="b">
         <v>1</v>
@@ -8031,10 +7972,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G38" s="29" t="b">
         <v>1</v>
@@ -8048,10 +7989,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G39" s="29" t="b">
         <v>1</v>
@@ -8065,10 +8006,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G40" s="29" t="b">
         <v>1</v>
@@ -8082,10 +8023,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G41" s="29" t="b">
         <v>1</v>
@@ -8099,10 +8040,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G42" s="29" t="b">
         <v>1</v>
@@ -8116,10 +8057,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G43" s="29" t="b">
         <v>1</v>
@@ -8133,10 +8074,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G44" s="29" t="b">
         <v>1</v>
@@ -8150,10 +8091,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G45" s="29" t="b">
         <v>1</v>
@@ -8167,10 +8108,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="G46" s="29" t="b">
         <v>1</v>
@@ -8184,10 +8125,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="G47" s="29" t="b">
         <v>1</v>
@@ -8201,10 +8142,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G48" s="29" t="b">
         <v>1</v>
@@ -8218,10 +8159,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G49" s="29" t="b">
         <v>1</v>
@@ -8235,10 +8176,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="G50" s="29" t="b">
         <v>1</v>
@@ -8252,10 +8193,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G51" s="29" t="b">
         <v>1</v>
@@ -8269,10 +8210,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G52" s="29" t="b">
         <v>1</v>
@@ -8286,10 +8227,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="29" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G53" s="29" t="b">
         <v>1</v>
@@ -8303,10 +8244,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G54" s="29" t="b">
         <v>1</v>
@@ -8320,10 +8261,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G55" s="29" t="b">
         <v>1</v>
@@ -8337,10 +8278,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G56" s="29" t="b">
         <v>1</v>
@@ -8354,10 +8295,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="29" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G57" s="29" t="b">
         <v>1</v>
@@ -8371,10 +8312,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="29" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="G58" s="29" t="b">
         <v>1</v>
@@ -8388,10 +8329,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="29" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="G59" s="29" t="b">
         <v>1</v>
@@ -8405,10 +8346,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="G60" s="29" t="b">
         <v>1</v>
@@ -8422,10 +8363,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G61" s="29" t="b">
         <v>1</v>
@@ -8439,10 +8380,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D62" s="29" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G62" s="29" t="b">
         <v>1</v>
@@ -8456,10 +8397,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D63" s="29" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G63" s="29" t="b">
         <v>1</v>
@@ -8473,10 +8414,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G64" s="29" t="b">
         <v>1</v>
@@ -8490,10 +8431,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G65" s="29" t="b">
         <v>1</v>
@@ -8507,10 +8448,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="29" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G66" s="29" t="b">
         <v>1</v>
@@ -8524,10 +8465,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D67" s="29" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="G67" s="29" t="b">
         <v>1</v>
@@ -8541,10 +8482,10 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D68" s="29" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G68" s="29" t="b">
         <v>1</v>
@@ -8558,10 +8499,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G69" s="29" t="b">
         <v>1</v>
@@ -8575,10 +8516,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G70" s="29" t="b">
         <v>1</v>
@@ -8592,10 +8533,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G71" s="29" t="b">
         <v>1</v>
@@ -8609,10 +8550,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G72" s="29" t="b">
         <v>1</v>
@@ -8626,10 +8567,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G73" s="29" t="b">
         <v>1</v>
@@ -8643,10 +8584,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D74" s="29" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G74" s="29" t="b">
         <v>1</v>
@@ -8660,10 +8601,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="29" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G75" s="29" t="b">
         <v>1</v>
@@ -8677,10 +8618,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D76" s="29" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G76" s="29" t="b">
         <v>1</v>
@@ -8694,10 +8635,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D77" s="29" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G77" s="29" t="b">
         <v>1</v>
@@ -8711,10 +8652,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G78" s="29" t="b">
         <v>1</v>
@@ -8728,10 +8669,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G79" s="29" t="b">
         <v>1</v>
@@ -8745,10 +8686,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G80" s="29" t="b">
         <v>1</v>
@@ -8762,10 +8703,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G81" s="29" t="b">
         <v>1</v>
@@ -8779,10 +8720,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G82" s="29" t="b">
         <v>1</v>
@@ -8796,10 +8737,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="G83" s="29" t="b">
         <v>1</v>
@@ -8813,10 +8754,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="29" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G84" s="29" t="b">
         <v>1</v>
@@ -8830,10 +8771,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G85" s="29" t="b">
         <v>1</v>
@@ -8847,10 +8788,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="29" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G86" s="29" t="b">
         <v>1</v>
@@ -8864,10 +8805,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="29" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D87" s="29" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G87" s="29" t="b">
         <v>1</v>
@@ -8881,10 +8822,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="29" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D88" s="29" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G88" s="29" t="b">
         <v>1</v>
@@ -8898,10 +8839,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="29" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D89" s="29" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G89" s="29" t="b">
         <v>1</v>
@@ -8915,10 +8856,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="29" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D90" s="29" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G90" s="29" t="b">
         <v>1</v>
@@ -8932,10 +8873,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="29" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="G91" s="29" t="b">
         <v>1</v>
@@ -8949,10 +8890,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="29" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D92" s="29" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G92" s="29" t="b">
         <v>1</v>
@@ -8966,10 +8907,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="29" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D93" s="29" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G93" s="29" t="b">
         <v>1</v>
@@ -8983,10 +8924,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="29" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G94" s="29" t="b">
         <v>1</v>
@@ -9000,10 +8941,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G95" s="29" t="b">
         <v>1</v>
@@ -9017,10 +8958,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G96" s="29" t="b">
         <v>1</v>
@@ -9034,10 +8975,10 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="29" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G97" s="29" t="b">
         <v>1</v>
@@ -9051,10 +8992,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="29" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G98" s="29" t="b">
         <v>1</v>
@@ -9068,10 +9009,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="29" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G99" s="29" t="b">
         <v>1</v>
@@ -9085,10 +9026,10 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G100" s="29" t="b">
         <v>1</v>
@@ -9102,10 +9043,10 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G101" s="29" t="b">
         <v>1</v>
@@ -9119,10 +9060,10 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D102" s="29" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G102" s="29" t="b">
         <v>1</v>
@@ -9136,10 +9077,10 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D103" s="29" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G103" s="29" t="b">
         <v>1</v>
@@ -9153,10 +9094,10 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="29" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D104" s="29" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G104" s="29" t="b">
         <v>1</v>
@@ -9170,10 +9111,10 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="29" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D105" s="29" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="G105" s="29" t="b">
         <v>1</v>
@@ -9187,10 +9128,10 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="29" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D106" s="29" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G106" s="29" t="b">
         <v>1</v>
@@ -9204,10 +9145,10 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="29" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D107" s="29" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G107" s="29" t="b">
         <v>1</v>
@@ -9221,10 +9162,10 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="29" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D108" s="29" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G108" s="29" t="b">
         <v>1</v>
@@ -9238,10 +9179,10 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="29" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D109" s="29" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="G109" s="29" t="b">
         <v>1</v>
@@ -9255,10 +9196,10 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="29" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D110" s="29" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="G110" s="29" t="b">
         <v>1</v>
@@ -9272,10 +9213,10 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="29" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D111" s="29" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G111" s="29" t="b">
         <v>1</v>
@@ -9289,10 +9230,10 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="29" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D112" s="29" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G112" s="29" t="b">
         <v>1</v>
@@ -9306,10 +9247,10 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="29" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D113" s="29" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G113" s="29" t="b">
         <v>1</v>
@@ -9323,10 +9264,10 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="29" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D114" s="29" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G114" s="29" t="b">
         <v>1</v>
@@ -9340,10 +9281,10 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="29" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D115" s="29" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G115" s="29" t="b">
         <v>1</v>
@@ -9357,10 +9298,10 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="29" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D116" s="29" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G116" s="29" t="b">
         <v>1</v>
@@ -9374,10 +9315,10 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="29" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D117" s="29" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G117" s="29" t="b">
         <v>1</v>
@@ -9391,10 +9332,10 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="29" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D118" s="29" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="G118" s="29" t="b">
         <v>1</v>
@@ -9408,10 +9349,10 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="29" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D119" s="29" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G119" s="29" t="b">
         <v>1</v>
@@ -9425,10 +9366,10 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="29" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D120" s="29" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="G120" s="29" t="b">
         <v>1</v>
@@ -9442,10 +9383,10 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="29" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D121" s="29" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="G121" s="29" t="b">
         <v>1</v>
@@ -9459,10 +9400,10 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="29" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G122" s="29" t="b">
         <v>1</v>
@@ -9476,10 +9417,10 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="29" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D123" s="29" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G123" s="29" t="b">
         <v>1</v>
@@ -9493,10 +9434,10 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D124" s="29" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="G124" s="29" t="b">
         <v>1</v>
@@ -9510,10 +9451,10 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="29" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D125" s="29" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="G125" s="29" t="b">
         <v>1</v>
@@ -9527,10 +9468,10 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="29" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D126" s="29" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="G126" s="29" t="b">
         <v>1</v>
@@ -9544,10 +9485,10 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="29" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D127" s="29" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G127" s="29" t="b">
         <v>1</v>
@@ -9561,10 +9502,10 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="29" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D128" s="29" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="G128" s="29" t="b">
         <v>1</v>
@@ -9578,10 +9519,10 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="29" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D129" s="29" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="G129" s="29" t="b">
         <v>1</v>
@@ -9595,10 +9536,10 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="29" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="G130" s="29" t="b">
         <v>1</v>
@@ -9612,10 +9553,10 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="29" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D131" s="29" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G131" s="29" t="b">
         <v>1</v>
@@ -9629,10 +9570,10 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="29" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G132" s="29" t="b">
         <v>1</v>
@@ -9646,10 +9587,10 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="29" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G133" s="29" t="b">
         <v>1</v>
@@ -9663,10 +9604,10 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="29" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="G134" s="29" t="b">
         <v>1</v>
@@ -9680,10 +9621,10 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="29" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D135" s="29" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G135" s="29" t="b">
         <v>1</v>
@@ -9697,10 +9638,10 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="29" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G136" s="29" t="b">
         <v>1</v>
@@ -9714,10 +9655,10 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="29" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D137" s="29" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G137" s="29" t="b">
         <v>1</v>
@@ -9731,10 +9672,10 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="29" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D138" s="29" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="G138" s="29" t="b">
         <v>1</v>
@@ -9748,10 +9689,10 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="29" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D139" s="29" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G139" s="29" t="b">
         <v>1</v>
@@ -9765,10 +9706,10 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="29" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D140" s="29" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G140" s="29" t="b">
         <v>1</v>
@@ -9782,10 +9723,10 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="29" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D141" s="29" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="G141" s="29" t="b">
         <v>1</v>
@@ -9799,10 +9740,10 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="29" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="G142" s="29" t="b">
         <v>1</v>
@@ -9816,10 +9757,10 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="29" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D143" s="29" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G143" s="29" t="b">
         <v>1</v>
@@ -9833,10 +9774,10 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="29" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D144" s="29" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="G144" s="29" t="b">
         <v>1</v>
@@ -9850,10 +9791,10 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="29" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D145" s="29" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G145" s="29" t="b">
         <v>1</v>
@@ -9867,10 +9808,10 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="29" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="G146" s="29" t="b">
         <v>1</v>
@@ -9884,10 +9825,10 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="29" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G147" s="29" t="b">
         <v>1</v>
@@ -9901,10 +9842,10 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="29" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="G148" s="29" t="b">
         <v>1</v>
@@ -9918,10 +9859,10 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="29" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="G149" s="29" t="b">
         <v>1</v>
@@ -9935,10 +9876,10 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="29" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="G150" s="29" t="b">
         <v>1</v>
@@ -9952,10 +9893,10 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="29" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D151" s="29" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="G151" s="29" t="b">
         <v>1</v>
@@ -9969,10 +9910,10 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="29" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D152" s="29" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G152" s="29" t="b">
         <v>1</v>
@@ -9986,10 +9927,10 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="29" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D153" s="29" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="G153" s="29" t="b">
         <v>1</v>
@@ -10003,10 +9944,10 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="29" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D154" s="29" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="G154" s="29" t="b">
         <v>1</v>
@@ -10020,10 +9961,10 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="29" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D155" s="29" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="G155" s="29" t="b">
         <v>1</v>
@@ -10037,10 +9978,10 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="29" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D156" s="29" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="G156" s="29" t="b">
         <v>1</v>
@@ -10054,10 +9995,10 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="29" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D157" s="29" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="G157" s="29" t="b">
         <v>1</v>
@@ -10071,10 +10012,10 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="29" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D158" s="29" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="G158" s="29" t="b">
         <v>1</v>
@@ -10088,10 +10029,10 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D159" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G159" s="29" t="b">
         <v>1</v>
@@ -10105,10 +10046,10 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="29" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D160" s="29" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G160" s="29" t="b">
         <v>1</v>
@@ -10122,10 +10063,10 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="29" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D161" s="29" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="G161" s="29" t="b">
         <v>1</v>
@@ -10139,10 +10080,10 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="29" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D162" s="29" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="G162" s="29" t="b">
         <v>1</v>
@@ -10156,10 +10097,10 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D163" s="29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G163" s="29" t="b">
         <v>1</v>
@@ -10173,10 +10114,10 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="29" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D164" s="29" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="G164" s="29" t="b">
         <v>1</v>
@@ -10190,10 +10131,10 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="29" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D165" s="29" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G165" s="29" t="b">
         <v>1</v>
@@ -10207,10 +10148,10 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="29" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D166" s="29" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G166" s="29" t="b">
         <v>1</v>
@@ -10224,10 +10165,10 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="29" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="D167" s="29" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G167" s="29" t="b">
         <v>1</v>
@@ -10241,10 +10182,10 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="29" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D168" s="29" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="G168" s="29" t="b">
         <v>1</v>
@@ -10258,10 +10199,10 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="29" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D169" s="29" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G169" s="29" t="b">
         <v>1</v>
@@ -10275,10 +10216,10 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="29" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D170" s="29" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="G170" s="29" t="b">
         <v>1</v>
@@ -10292,10 +10233,10 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="29" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D171" s="29" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G171" s="29" t="b">
         <v>1</v>
@@ -10309,10 +10250,10 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="29" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D172" s="29" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G172" s="29" t="b">
         <v>1</v>
@@ -10326,10 +10267,10 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="29" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D173" s="29" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="G173" s="29" t="b">
         <v>1</v>
@@ -10343,10 +10284,10 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="29" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D174" s="29" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="G174" s="29" t="b">
         <v>1</v>
@@ -10360,10 +10301,10 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="29" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D175" s="29" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G175" s="29" t="b">
         <v>1</v>
@@ -10377,10 +10318,10 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="29" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D176" s="29" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G176" s="29" t="b">
         <v>1</v>
@@ -10394,10 +10335,10 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="29" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D177" s="29" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G177" s="29" t="b">
         <v>1</v>
@@ -10411,10 +10352,10 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="29" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D178" s="29" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="G178" s="29" t="b">
         <v>1</v>
@@ -10428,10 +10369,10 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="29" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D179" s="29" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G179" s="29" t="b">
         <v>1</v>
@@ -10445,10 +10386,10 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="29" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D180" s="29" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G180" s="29" t="b">
         <v>1</v>
@@ -10462,10 +10403,10 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="29" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D181" s="29" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G181" s="29" t="b">
         <v>1</v>
@@ -10479,10 +10420,10 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="29" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D182" s="29" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G182" s="29" t="b">
         <v>1</v>
@@ -10496,10 +10437,10 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="29" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D183" s="29" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G183" s="29" t="b">
         <v>1</v>
@@ -10513,10 +10454,10 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="29" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D184" s="29" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G184" s="29" t="b">
         <v>1</v>
@@ -10530,10 +10471,10 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="29" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D185" s="29" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G185" s="29" t="b">
         <v>1</v>
@@ -10547,10 +10488,10 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="29" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D186" s="29" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G186" s="29" t="b">
         <v>1</v>
@@ -10564,10 +10505,10 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="29" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D187" s="29" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G187" s="29" t="b">
         <v>1</v>
@@ -10581,10 +10522,10 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="29" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D188" s="29" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="G188" s="29" t="b">
         <v>1</v>
@@ -10598,10 +10539,10 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="29" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D189" s="29" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G189" s="29" t="b">
         <v>1</v>
@@ -10615,10 +10556,10 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="29" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D190" s="29" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="G190" s="29" t="b">
         <v>1</v>
@@ -10632,10 +10573,10 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D191" s="29" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G191" s="29" t="b">
         <v>1</v>
@@ -10649,10 +10590,10 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="29" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D192" s="29" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G192" s="29" t="b">
         <v>1</v>
@@ -10666,10 +10607,10 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="29" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D193" s="29" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="G193" s="29" t="b">
         <v>1</v>
@@ -10683,10 +10624,10 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="29" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D194" s="29" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G194" s="29" t="b">
         <v>1</v>
@@ -10700,10 +10641,10 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="29" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D195" s="29" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G195" s="29" t="b">
         <v>1</v>
@@ -10717,10 +10658,10 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="29" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D196" s="29" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="G196" s="29" t="b">
         <v>1</v>
@@ -10734,10 +10675,10 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="29" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D197" s="29" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G197" s="29" t="b">
         <v>1</v>
@@ -10751,10 +10692,10 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="29" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D198" s="29" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G198" s="29" t="b">
         <v>1</v>
@@ -10768,10 +10709,10 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="29" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D199" s="29" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="G199" s="29" t="b">
         <v>1</v>
@@ -10785,10 +10726,10 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="29" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="G200" s="29" t="b">
         <v>1</v>
@@ -10802,10 +10743,10 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="29" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D201" s="29" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="G201" s="29" t="b">
         <v>1</v>
@@ -10819,10 +10760,10 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="29" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D202" s="29" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G202" s="29" t="b">
         <v>1</v>
@@ -10836,10 +10777,10 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="29" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G203" s="29" t="b">
         <v>1</v>
@@ -10853,10 +10794,10 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="29" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G204" s="29" t="b">
         <v>1</v>
@@ -10870,10 +10811,10 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="G205" s="29" t="b">
         <v>1</v>
@@ -10887,10 +10828,10 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="29" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D206" s="29" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G206" s="29" t="b">
         <v>1</v>
@@ -10904,10 +10845,10 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="29" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G207" s="29" t="b">
         <v>1</v>
@@ -10921,10 +10862,10 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="29" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G208" s="29" t="b">
         <v>1</v>
@@ -10938,10 +10879,10 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="29" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="G209" s="29" t="b">
         <v>1</v>
@@ -10955,10 +10896,10 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="29" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="G210" s="29" t="b">
         <v>1</v>
@@ -10972,10 +10913,10 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="29" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G211" s="29" t="b">
         <v>1</v>
@@ -10989,10 +10930,10 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="29" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="G212" s="29" t="b">
         <v>1</v>
@@ -11006,10 +10947,10 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="29" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G213" s="29" t="b">
         <v>1</v>
@@ -11023,10 +10964,10 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="29" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G214" s="29" t="b">
         <v>1</v>
@@ -11040,10 +10981,10 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="29" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G215" s="29" t="b">
         <v>1</v>
@@ -11057,10 +10998,10 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="29" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="G216" s="29" t="b">
         <v>1</v>
@@ -11074,10 +11015,10 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="29" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="G217" s="29" t="b">
         <v>1</v>
@@ -11091,10 +11032,10 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="29" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="G218" s="29" t="b">
         <v>1</v>
@@ -11108,10 +11049,10 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="29" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="G219" s="29" t="b">
         <v>1</v>
@@ -11125,10 +11066,10 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="29" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="G220" s="29" t="b">
         <v>1</v>
@@ -11142,10 +11083,10 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="29" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G221" s="29" t="b">
         <v>1</v>
@@ -11154,6 +11095,23 @@
         <v>1</v>
       </c>
       <c r="I221" s="29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A222" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="D222" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="G222" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H222" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I222" s="29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -11671,10 +11629,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11698,124 +11656,137 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
+    <row r="3" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>479</v>
+      </c>
+      <c r="B3" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>221</v>
+        <v>477</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
         <v>245</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="52"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
         <v>247</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added option for hourly data argument for BTAPResults measure
</commit_message>
<xml_diff>
--- a/projects/NECB_QA_QC.xlsx
+++ b/projects/NECB_QA_QC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5790" windowWidth="19440" windowHeight="4725" tabRatio="469" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="5790" windowWidth="19440" windowHeight="4725" tabRatio="469" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="484">
   <si>
     <t>type</t>
   </si>
@@ -792,15 +792,6 @@
     <t>argument</t>
   </si>
   <si>
-    <t>Select Vintage</t>
-  </si>
-  <si>
-    <t>90.1-2010</t>
-  </si>
-  <si>
-    <t>["90.1-2010"]</t>
-  </si>
-  <si>
     <t>ViewModel</t>
   </si>
   <si>
@@ -1486,6 +1477,18 @@
   </si>
   <si>
     <t>btapresults.btap_results_json_zip</t>
+  </si>
+  <si>
+    <t>Generate Hourly Report.</t>
+  </si>
+  <si>
+    <t>generate_hourly_report</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>FaLsE</t>
   </si>
 </sst>
 </file>
@@ -3955,7 +3958,7 @@
     <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4068,7 +4071,6 @@
     <xf numFmtId="0" fontId="29" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6377,7 +6379,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>157</v>
@@ -6388,7 +6390,7 @@
         <v>75</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>77</v>
@@ -6494,7 +6496,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="29" t="s">
@@ -6784,8 +6786,8 @@
   </sheetPr>
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -6840,14 +6842,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="61" t="s">
+      <c r="U1" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -6999,7 +7001,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="Q5" s="53"/>
       <c r="R5" s="53" t="s">
@@ -7131,7 +7133,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="43" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="Q8" s="53"/>
       <c r="R8" s="53" t="s">
@@ -7139,64 +7141,50 @@
       </c>
     </row>
     <row r="9" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="53" t="s">
-        <v>250</v>
-      </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53" t="s">
+      <c r="A9" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>252</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="E9" s="53" t="s">
-        <v>197</v>
-      </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53" t="s">
-        <v>188</v>
-      </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="60" t="s">
-        <v>252</v>
-      </c>
-      <c r="J9" s="60"/>
-      <c r="K9" s="53">
-        <v>1</v>
-      </c>
-      <c r="L9" s="53">
-        <v>1</v>
-      </c>
-      <c r="M9" s="53">
-        <v>1</v>
-      </c>
-      <c r="N9" s="53">
-        <v>1</v>
-      </c>
-      <c r="O9" s="53">
-        <v>1</v>
-      </c>
-      <c r="P9" s="53" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53" t="s">
-        <v>195</v>
-      </c>
+      <c r="E9" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
     </row>
     <row r="10" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="b">
         <v>1</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>255</v>
+        <v>214</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>255</v>
+        <v>214</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>41</v>
+        <v>215</v>
       </c>
       <c r="F10" s="58"/>
       <c r="G10" s="58"/>
@@ -7212,47 +7200,51 @@
       <c r="Q10" s="58"/>
       <c r="R10" s="58"/>
     </row>
-    <row r="11" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>215</v>
-      </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
+    <row r="11" spans="1:26" s="46" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53" t="s">
+        <v>480</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>481</v>
+      </c>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53" t="s">
+        <v>482</v>
+      </c>
+      <c r="H11" s="53"/>
+      <c r="I11" s="56" t="s">
+        <v>483</v>
+      </c>
+      <c r="J11" s="53"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="53" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA7"/>
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:A11">
+  <conditionalFormatting sqref="A9:A10">
     <cfRule type="cellIs" dxfId="3" priority="126" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A11">
+  <conditionalFormatting sqref="A9:A10">
     <cfRule type="cellIs" dxfId="2" priority="125" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -7276,7 +7268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I223" sqref="I223"/>
     </sheetView>
@@ -7394,10 +7386,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G4" s="29" t="b">
         <v>1</v>
@@ -7411,10 +7403,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G5" s="29" t="b">
         <v>1</v>
@@ -7428,10 +7420,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G6" s="29" t="b">
         <v>1</v>
@@ -7445,10 +7437,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G7" s="29" t="b">
         <v>1</v>
@@ -7462,10 +7454,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G8" s="29" t="b">
         <v>1</v>
@@ -7479,10 +7471,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G9" s="29" t="b">
         <v>1</v>
@@ -7496,10 +7488,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G10" s="29" t="b">
         <v>1</v>
@@ -7513,10 +7505,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G11" s="29" t="b">
         <v>1</v>
@@ -7530,10 +7522,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G12" s="29" t="b">
         <v>1</v>
@@ -7547,10 +7539,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G13" s="29" t="b">
         <v>1</v>
@@ -7564,10 +7556,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G14" s="29" t="b">
         <v>1</v>
@@ -7581,10 +7573,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G15" s="29" t="b">
         <v>1</v>
@@ -7598,10 +7590,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G16" s="29" t="b">
         <v>1</v>
@@ -7615,10 +7607,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G17" s="29" t="b">
         <v>1</v>
@@ -7632,10 +7624,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G18" s="29" t="b">
         <v>1</v>
@@ -7649,10 +7641,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G19" s="29" t="b">
         <v>1</v>
@@ -7666,10 +7658,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G20" s="29" t="b">
         <v>1</v>
@@ -7683,10 +7675,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G21" s="29" t="b">
         <v>1</v>
@@ -7700,10 +7692,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G22" s="29" t="b">
         <v>1</v>
@@ -7717,10 +7709,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G23" s="29" t="b">
         <v>1</v>
@@ -7734,10 +7726,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G24" s="29" t="b">
         <v>1</v>
@@ -7751,10 +7743,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G25" s="29" t="b">
         <v>1</v>
@@ -7768,10 +7760,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G26" s="29" t="b">
         <v>1</v>
@@ -7785,10 +7777,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G27" s="29" t="b">
         <v>1</v>
@@ -7802,10 +7794,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G28" s="29" t="b">
         <v>1</v>
@@ -7819,10 +7811,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G29" s="29" t="b">
         <v>1</v>
@@ -7836,10 +7828,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G30" s="29" t="b">
         <v>1</v>
@@ -7853,10 +7845,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G31" s="29" t="b">
         <v>1</v>
@@ -7870,10 +7862,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G32" s="29" t="b">
         <v>1</v>
@@ -7887,10 +7879,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G33" s="29" t="b">
         <v>1</v>
@@ -7904,10 +7896,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G34" s="29" t="b">
         <v>1</v>
@@ -7921,10 +7913,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G35" s="29" t="b">
         <v>1</v>
@@ -7938,10 +7930,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G36" s="29" t="b">
         <v>1</v>
@@ -7955,10 +7947,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G37" s="29" t="b">
         <v>1</v>
@@ -7972,10 +7964,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G38" s="29" t="b">
         <v>1</v>
@@ -7989,10 +7981,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G39" s="29" t="b">
         <v>1</v>
@@ -8006,10 +7998,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G40" s="29" t="b">
         <v>1</v>
@@ -8023,10 +8015,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G41" s="29" t="b">
         <v>1</v>
@@ -8040,10 +8032,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G42" s="29" t="b">
         <v>1</v>
@@ -8057,10 +8049,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G43" s="29" t="b">
         <v>1</v>
@@ -8074,10 +8066,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G44" s="29" t="b">
         <v>1</v>
@@ -8091,10 +8083,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G45" s="29" t="b">
         <v>1</v>
@@ -8108,10 +8100,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G46" s="29" t="b">
         <v>1</v>
@@ -8125,10 +8117,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G47" s="29" t="b">
         <v>1</v>
@@ -8142,10 +8134,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G48" s="29" t="b">
         <v>1</v>
@@ -8159,10 +8151,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G49" s="29" t="b">
         <v>1</v>
@@ -8176,10 +8168,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G50" s="29" t="b">
         <v>1</v>
@@ -8193,10 +8185,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G51" s="29" t="b">
         <v>1</v>
@@ -8210,10 +8202,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G52" s="29" t="b">
         <v>1</v>
@@ -8227,10 +8219,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="29" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G53" s="29" t="b">
         <v>1</v>
@@ -8244,10 +8236,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G54" s="29" t="b">
         <v>1</v>
@@ -8261,10 +8253,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G55" s="29" t="b">
         <v>1</v>
@@ -8278,10 +8270,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G56" s="29" t="b">
         <v>1</v>
@@ -8295,10 +8287,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="29" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G57" s="29" t="b">
         <v>1</v>
@@ -8312,10 +8304,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="29" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G58" s="29" t="b">
         <v>1</v>
@@ -8329,10 +8321,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="29" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G59" s="29" t="b">
         <v>1</v>
@@ -8346,10 +8338,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G60" s="29" t="b">
         <v>1</v>
@@ -8363,10 +8355,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="29" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G61" s="29" t="b">
         <v>1</v>
@@ -8380,10 +8372,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D62" s="29" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G62" s="29" t="b">
         <v>1</v>
@@ -8397,10 +8389,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D63" s="29" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G63" s="29" t="b">
         <v>1</v>
@@ -8414,10 +8406,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G64" s="29" t="b">
         <v>1</v>
@@ -8431,10 +8423,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G65" s="29" t="b">
         <v>1</v>
@@ -8448,10 +8440,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="29" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G66" s="29" t="b">
         <v>1</v>
@@ -8465,10 +8457,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D67" s="29" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G67" s="29" t="b">
         <v>1</v>
@@ -8482,10 +8474,10 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D68" s="29" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G68" s="29" t="b">
         <v>1</v>
@@ -8499,10 +8491,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G69" s="29" t="b">
         <v>1</v>
@@ -8516,10 +8508,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G70" s="29" t="b">
         <v>1</v>
@@ -8533,10 +8525,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G71" s="29" t="b">
         <v>1</v>
@@ -8550,10 +8542,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G72" s="29" t="b">
         <v>1</v>
@@ -8567,10 +8559,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G73" s="29" t="b">
         <v>1</v>
@@ -8584,10 +8576,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D74" s="29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G74" s="29" t="b">
         <v>1</v>
@@ -8601,10 +8593,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="29" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G75" s="29" t="b">
         <v>1</v>
@@ -8618,10 +8610,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D76" s="29" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G76" s="29" t="b">
         <v>1</v>
@@ -8635,10 +8627,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D77" s="29" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G77" s="29" t="b">
         <v>1</v>
@@ -8652,10 +8644,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G78" s="29" t="b">
         <v>1</v>
@@ -8669,10 +8661,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G79" s="29" t="b">
         <v>1</v>
@@ -8686,10 +8678,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G80" s="29" t="b">
         <v>1</v>
@@ -8703,10 +8695,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G81" s="29" t="b">
         <v>1</v>
@@ -8720,10 +8712,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G82" s="29" t="b">
         <v>1</v>
@@ -8737,10 +8729,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G83" s="29" t="b">
         <v>1</v>
@@ -8754,10 +8746,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="29" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G84" s="29" t="b">
         <v>1</v>
@@ -8771,10 +8763,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G85" s="29" t="b">
         <v>1</v>
@@ -8788,10 +8780,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G86" s="29" t="b">
         <v>1</v>
@@ -8805,10 +8797,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D87" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G87" s="29" t="b">
         <v>1</v>
@@ -8822,10 +8814,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="29" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D88" s="29" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G88" s="29" t="b">
         <v>1</v>
@@ -8839,10 +8831,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="29" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D89" s="29" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G89" s="29" t="b">
         <v>1</v>
@@ -8856,10 +8848,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="29" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D90" s="29" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G90" s="29" t="b">
         <v>1</v>
@@ -8873,10 +8865,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="29" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G91" s="29" t="b">
         <v>1</v>
@@ -8890,10 +8882,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="29" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D92" s="29" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G92" s="29" t="b">
         <v>1</v>
@@ -8907,10 +8899,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="29" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D93" s="29" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G93" s="29" t="b">
         <v>1</v>
@@ -8924,10 +8916,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="29" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G94" s="29" t="b">
         <v>1</v>
@@ -8941,10 +8933,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G95" s="29" t="b">
         <v>1</v>
@@ -8958,10 +8950,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G96" s="29" t="b">
         <v>1</v>
@@ -8975,10 +8967,10 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="29" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G97" s="29" t="b">
         <v>1</v>
@@ -8992,10 +8984,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="29" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G98" s="29" t="b">
         <v>1</v>
@@ -9009,10 +9001,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="29" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G99" s="29" t="b">
         <v>1</v>
@@ -9026,10 +9018,10 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G100" s="29" t="b">
         <v>1</v>
@@ -9043,10 +9035,10 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G101" s="29" t="b">
         <v>1</v>
@@ -9060,10 +9052,10 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D102" s="29" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G102" s="29" t="b">
         <v>1</v>
@@ -9077,10 +9069,10 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D103" s="29" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G103" s="29" t="b">
         <v>1</v>
@@ -9094,10 +9086,10 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="29" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D104" s="29" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G104" s="29" t="b">
         <v>1</v>
@@ -9111,10 +9103,10 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="29" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D105" s="29" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G105" s="29" t="b">
         <v>1</v>
@@ -9128,10 +9120,10 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="29" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D106" s="29" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G106" s="29" t="b">
         <v>1</v>
@@ -9145,10 +9137,10 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="29" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D107" s="29" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G107" s="29" t="b">
         <v>1</v>
@@ -9162,10 +9154,10 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="29" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D108" s="29" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G108" s="29" t="b">
         <v>1</v>
@@ -9179,10 +9171,10 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="29" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D109" s="29" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G109" s="29" t="b">
         <v>1</v>
@@ -9196,10 +9188,10 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="29" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D110" s="29" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G110" s="29" t="b">
         <v>1</v>
@@ -9213,10 +9205,10 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="29" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D111" s="29" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G111" s="29" t="b">
         <v>1</v>
@@ -9230,10 +9222,10 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="29" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D112" s="29" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G112" s="29" t="b">
         <v>1</v>
@@ -9247,10 +9239,10 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="29" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D113" s="29" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G113" s="29" t="b">
         <v>1</v>
@@ -9264,10 +9256,10 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="29" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D114" s="29" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G114" s="29" t="b">
         <v>1</v>
@@ -9281,10 +9273,10 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="29" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D115" s="29" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G115" s="29" t="b">
         <v>1</v>
@@ -9298,10 +9290,10 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="29" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D116" s="29" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G116" s="29" t="b">
         <v>1</v>
@@ -9315,10 +9307,10 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="29" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D117" s="29" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G117" s="29" t="b">
         <v>1</v>
@@ -9332,10 +9324,10 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="29" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D118" s="29" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G118" s="29" t="b">
         <v>1</v>
@@ -9349,10 +9341,10 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D119" s="29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G119" s="29" t="b">
         <v>1</v>
@@ -9366,10 +9358,10 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D120" s="29" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G120" s="29" t="b">
         <v>1</v>
@@ -9383,10 +9375,10 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="29" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D121" s="29" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G121" s="29" t="b">
         <v>1</v>
@@ -9400,10 +9392,10 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G122" s="29" t="b">
         <v>1</v>
@@ -9417,10 +9409,10 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="29" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D123" s="29" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G123" s="29" t="b">
         <v>1</v>
@@ -9434,10 +9426,10 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D124" s="29" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G124" s="29" t="b">
         <v>1</v>
@@ -9451,10 +9443,10 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="29" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D125" s="29" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G125" s="29" t="b">
         <v>1</v>
@@ -9468,10 +9460,10 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="29" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D126" s="29" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G126" s="29" t="b">
         <v>1</v>
@@ -9485,10 +9477,10 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="29" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D127" s="29" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G127" s="29" t="b">
         <v>1</v>
@@ -9502,10 +9494,10 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="29" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D128" s="29" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G128" s="29" t="b">
         <v>1</v>
@@ -9519,10 +9511,10 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="29" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D129" s="29" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G129" s="29" t="b">
         <v>1</v>
@@ -9536,10 +9528,10 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="29" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G130" s="29" t="b">
         <v>1</v>
@@ -9553,10 +9545,10 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="29" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D131" s="29" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G131" s="29" t="b">
         <v>1</v>
@@ -9570,10 +9562,10 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="29" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G132" s="29" t="b">
         <v>1</v>
@@ -9587,10 +9579,10 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="29" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G133" s="29" t="b">
         <v>1</v>
@@ -9604,10 +9596,10 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="29" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G134" s="29" t="b">
         <v>1</v>
@@ -9621,10 +9613,10 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="29" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D135" s="29" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G135" s="29" t="b">
         <v>1</v>
@@ -9638,10 +9630,10 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="29" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G136" s="29" t="b">
         <v>1</v>
@@ -9655,10 +9647,10 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="29" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D137" s="29" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G137" s="29" t="b">
         <v>1</v>
@@ -9672,10 +9664,10 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="29" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D138" s="29" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G138" s="29" t="b">
         <v>1</v>
@@ -9689,10 +9681,10 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="29" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D139" s="29" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G139" s="29" t="b">
         <v>1</v>
@@ -9706,10 +9698,10 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="29" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D140" s="29" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G140" s="29" t="b">
         <v>1</v>
@@ -9723,10 +9715,10 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="29" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D141" s="29" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G141" s="29" t="b">
         <v>1</v>
@@ -9740,10 +9732,10 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="29" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="G142" s="29" t="b">
         <v>1</v>
@@ -9757,10 +9749,10 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="29" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D143" s="29" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G143" s="29" t="b">
         <v>1</v>
@@ -9774,10 +9766,10 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="29" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D144" s="29" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G144" s="29" t="b">
         <v>1</v>
@@ -9791,10 +9783,10 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="29" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D145" s="29" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G145" s="29" t="b">
         <v>1</v>
@@ -9808,10 +9800,10 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="29" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G146" s="29" t="b">
         <v>1</v>
@@ -9825,10 +9817,10 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="29" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G147" s="29" t="b">
         <v>1</v>
@@ -9842,10 +9834,10 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="29" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G148" s="29" t="b">
         <v>1</v>
@@ -9859,10 +9851,10 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="29" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G149" s="29" t="b">
         <v>1</v>
@@ -9876,10 +9868,10 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="29" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G150" s="29" t="b">
         <v>1</v>
@@ -9893,10 +9885,10 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="29" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D151" s="29" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G151" s="29" t="b">
         <v>1</v>
@@ -9910,10 +9902,10 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="29" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D152" s="29" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="G152" s="29" t="b">
         <v>1</v>
@@ -9927,10 +9919,10 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="29" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D153" s="29" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G153" s="29" t="b">
         <v>1</v>
@@ -9944,10 +9936,10 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="29" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D154" s="29" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G154" s="29" t="b">
         <v>1</v>
@@ -9961,10 +9953,10 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="29" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D155" s="29" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="G155" s="29" t="b">
         <v>1</v>
@@ -9978,10 +9970,10 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="29" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D156" s="29" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G156" s="29" t="b">
         <v>1</v>
@@ -9995,10 +9987,10 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="29" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D157" s="29" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G157" s="29" t="b">
         <v>1</v>
@@ -10012,10 +10004,10 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="29" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D158" s="29" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G158" s="29" t="b">
         <v>1</v>
@@ -10029,10 +10021,10 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="29" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D159" s="29" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G159" s="29" t="b">
         <v>1</v>
@@ -10046,10 +10038,10 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="29" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D160" s="29" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G160" s="29" t="b">
         <v>1</v>
@@ -10063,10 +10055,10 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="29" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D161" s="29" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G161" s="29" t="b">
         <v>1</v>
@@ -10080,10 +10072,10 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="29" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D162" s="29" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G162" s="29" t="b">
         <v>1</v>
@@ -10097,10 +10089,10 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="29" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D163" s="29" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G163" s="29" t="b">
         <v>1</v>
@@ -10114,10 +10106,10 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="29" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D164" s="29" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G164" s="29" t="b">
         <v>1</v>
@@ -10131,10 +10123,10 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="29" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D165" s="29" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G165" s="29" t="b">
         <v>1</v>
@@ -10148,10 +10140,10 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="29" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D166" s="29" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="G166" s="29" t="b">
         <v>1</v>
@@ -10165,10 +10157,10 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="29" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D167" s="29" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G167" s="29" t="b">
         <v>1</v>
@@ -10182,10 +10174,10 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="29" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D168" s="29" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G168" s="29" t="b">
         <v>1</v>
@@ -10199,10 +10191,10 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="29" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D169" s="29" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G169" s="29" t="b">
         <v>1</v>
@@ -10216,10 +10208,10 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="29" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D170" s="29" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G170" s="29" t="b">
         <v>1</v>
@@ -10233,10 +10225,10 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="29" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D171" s="29" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G171" s="29" t="b">
         <v>1</v>
@@ -10250,10 +10242,10 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="29" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D172" s="29" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G172" s="29" t="b">
         <v>1</v>
@@ -10267,10 +10259,10 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="29" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D173" s="29" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G173" s="29" t="b">
         <v>1</v>
@@ -10284,10 +10276,10 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="29" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D174" s="29" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G174" s="29" t="b">
         <v>1</v>
@@ -10301,10 +10293,10 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="29" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D175" s="29" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G175" s="29" t="b">
         <v>1</v>
@@ -10318,10 +10310,10 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="29" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D176" s="29" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="G176" s="29" t="b">
         <v>1</v>
@@ -10335,10 +10327,10 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="29" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D177" s="29" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G177" s="29" t="b">
         <v>1</v>
@@ -10352,10 +10344,10 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="29" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D178" s="29" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G178" s="29" t="b">
         <v>1</v>
@@ -10369,10 +10361,10 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="29" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D179" s="29" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G179" s="29" t="b">
         <v>1</v>
@@ -10386,10 +10378,10 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="29" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D180" s="29" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G180" s="29" t="b">
         <v>1</v>
@@ -10403,10 +10395,10 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="29" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D181" s="29" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G181" s="29" t="b">
         <v>1</v>
@@ -10420,10 +10412,10 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="29" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D182" s="29" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G182" s="29" t="b">
         <v>1</v>
@@ -10437,10 +10429,10 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="29" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D183" s="29" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="G183" s="29" t="b">
         <v>1</v>
@@ -10454,10 +10446,10 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="29" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D184" s="29" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="G184" s="29" t="b">
         <v>1</v>
@@ -10471,10 +10463,10 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="29" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D185" s="29" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G185" s="29" t="b">
         <v>1</v>
@@ -10488,10 +10480,10 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="29" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D186" s="29" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G186" s="29" t="b">
         <v>1</v>
@@ -10505,10 +10497,10 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="29" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D187" s="29" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="G187" s="29" t="b">
         <v>1</v>
@@ -10522,10 +10514,10 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="29" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D188" s="29" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G188" s="29" t="b">
         <v>1</v>
@@ -10539,10 +10531,10 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="29" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D189" s="29" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G189" s="29" t="b">
         <v>1</v>
@@ -10556,10 +10548,10 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="29" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D190" s="29" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="G190" s="29" t="b">
         <v>1</v>
@@ -10573,10 +10565,10 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D191" s="29" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="G191" s="29" t="b">
         <v>1</v>
@@ -10590,10 +10582,10 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="29" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D192" s="29" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G192" s="29" t="b">
         <v>1</v>
@@ -10607,10 +10599,10 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="29" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D193" s="29" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="G193" s="29" t="b">
         <v>1</v>
@@ -10624,10 +10616,10 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="29" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D194" s="29" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="G194" s="29" t="b">
         <v>1</v>
@@ -10641,10 +10633,10 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D195" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G195" s="29" t="b">
         <v>1</v>
@@ -10658,10 +10650,10 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="29" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D196" s="29" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G196" s="29" t="b">
         <v>1</v>
@@ -10675,10 +10667,10 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="29" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D197" s="29" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G197" s="29" t="b">
         <v>1</v>
@@ -10692,10 +10684,10 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="29" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D198" s="29" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G198" s="29" t="b">
         <v>1</v>
@@ -10709,10 +10701,10 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="29" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D199" s="29" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G199" s="29" t="b">
         <v>1</v>
@@ -10726,10 +10718,10 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="G200" s="29" t="b">
         <v>1</v>
@@ -10743,10 +10735,10 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="29" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D201" s="29" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G201" s="29" t="b">
         <v>1</v>
@@ -10760,10 +10752,10 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="29" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D202" s="29" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G202" s="29" t="b">
         <v>1</v>
@@ -10777,10 +10769,10 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="29" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="G203" s="29" t="b">
         <v>1</v>
@@ -10794,10 +10786,10 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="29" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G204" s="29" t="b">
         <v>1</v>
@@ -10811,10 +10803,10 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="G205" s="29" t="b">
         <v>1</v>
@@ -10828,10 +10820,10 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="29" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D206" s="29" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G206" s="29" t="b">
         <v>1</v>
@@ -10845,10 +10837,10 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="29" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="G207" s="29" t="b">
         <v>1</v>
@@ -10862,10 +10854,10 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="29" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G208" s="29" t="b">
         <v>1</v>
@@ -10879,10 +10871,10 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="29" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="G209" s="29" t="b">
         <v>1</v>
@@ -10896,10 +10888,10 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="29" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G210" s="29" t="b">
         <v>1</v>
@@ -10913,10 +10905,10 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="29" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G211" s="29" t="b">
         <v>1</v>
@@ -10930,10 +10922,10 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="29" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G212" s="29" t="b">
         <v>1</v>
@@ -10947,10 +10939,10 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="29" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G213" s="29" t="b">
         <v>1</v>
@@ -10964,10 +10956,10 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="29" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G214" s="29" t="b">
         <v>1</v>
@@ -10981,10 +10973,10 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="29" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G215" s="29" t="b">
         <v>1</v>
@@ -10998,10 +10990,10 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="29" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G216" s="29" t="b">
         <v>1</v>
@@ -11015,10 +11007,10 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="29" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G217" s="29" t="b">
         <v>1</v>
@@ -11032,10 +11024,10 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="29" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="G218" s="29" t="b">
         <v>1</v>
@@ -11049,10 +11041,10 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="29" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G219" s="29" t="b">
         <v>1</v>
@@ -11066,10 +11058,10 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="29" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G220" s="29" t="b">
         <v>1</v>
@@ -11083,10 +11075,10 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="29" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G221" s="29" t="b">
         <v>1</v>
@@ -11100,10 +11092,10 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="29" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D222" s="29" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G222" s="29" t="b">
         <v>1</v>
@@ -11658,18 +11650,18 @@
     </row>
     <row r="3" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="B4" t="s">
         <v>477</v>
-      </c>
-      <c r="B4" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>